<commit_message>
smal changes made for chat
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="83">
   <si>
     <t>Play song</t>
   </si>
@@ -217,12 +217,6 @@
     <t>Spike on binding</t>
   </si>
   <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>Documenter</t>
-  </si>
-  <si>
     <t>Create playlist</t>
   </si>
   <si>
@@ -269,6 +263,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
@@ -304,10 +307,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -324,6 +330,1102 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="lv-LV"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.3803149606299209E-2"/>
+          <c:y val="3.7037037037037035E-2"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sprint 1'!$S$2:$S$14</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sprint 1'!$S$2:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sprint 1'!$Q$2:$Q$34</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sprint 1'!$Q$2:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-7559-492D-A8CB-4D0B2A504E32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1'!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sprint 1'!$S$2:$S$14</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sprint 1'!$S$2:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sprint 1'!$R$2:$R$34</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sprint 1'!$R$2:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-7559-492D-A8CB-4D0B2A504E32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="488277248"/>
+        <c:axId val="488277576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="488277248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="lv-LV"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488277576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488277576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="lv-LV"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488277248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="lv-LV"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>299358</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>131989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>312964</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>17689</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramma 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F655AD2-89FA-4209-B3BA-24E168D91292}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -800,7 +1902,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
         <v>42</v>
@@ -927,7 +2029,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
         <v>42</v>
@@ -938,7 +2040,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
@@ -949,7 +2051,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
         <v>42</v>
@@ -963,7 +2065,7 @@
         <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -974,7 +2076,7 @@
         <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1004,7 +2106,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
         <v>42</v>
@@ -1015,7 +2117,7 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
         <v>42</v>
@@ -1026,7 +2128,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
         <v>42</v>
@@ -1037,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
@@ -1048,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
         <v>42</v>
@@ -1059,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
         <v>42</v>
@@ -1073,7 +2175,7 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1095,7 +2197,7 @@
         <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1105,19 +2207,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1136,8 +2240,23 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1153,11 +2272,28 @@
       <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <f>M34-SUM(M2:M5)</f>
+        <v>104</v>
+      </c>
+      <c r="R2">
+        <f>N34-SUM(N2:N5)</f>
+        <v>113</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1173,11 +2309,28 @@
       <c r="E3" t="s">
         <v>50</v>
       </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f>Q2-SUM(M6)</f>
+        <v>101</v>
+      </c>
+      <c r="R3">
+        <f>R2-SUM(N6)</f>
+        <v>110</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1193,11 +2346,28 @@
       <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <f>Q3-SUM(M7:M8)</f>
+        <v>97</v>
+      </c>
+      <c r="R4">
+        <f>R3-SUM(N7:N8)</f>
+        <v>105</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1213,11 +2383,28 @@
       <c r="E5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <f>Q4-SUM(M9:M10)</f>
+        <v>91</v>
+      </c>
+      <c r="R5">
+        <f>R4-SUM(N9:N10)</f>
+        <v>99</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1233,11 +2420,28 @@
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <f>Q5-SUM(M11:M12)</f>
+        <v>86</v>
+      </c>
+      <c r="R6">
+        <f>R5-SUM(N11:N12)</f>
+        <v>95</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1253,11 +2457,28 @@
       <c r="E7" t="s">
         <v>50</v>
       </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <f>Q6-SUM(M13:M15)</f>
+        <v>77</v>
+      </c>
+      <c r="R7">
+        <f>R6-SUM(N13:N15)</f>
+        <v>86</v>
+      </c>
+      <c r="S7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1276,8 +2497,28 @@
       <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <f>Q7-SUM(M16:M17)</f>
+        <v>68</v>
+      </c>
+      <c r="R8">
+        <f>R7-SUM(N16:N17)</f>
+        <v>72</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1296,8 +2537,28 @@
       <c r="F9" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <f>Q8-SUM(M18)</f>
+        <v>65</v>
+      </c>
+      <c r="R9">
+        <f>R8-SUM(N18)</f>
+        <v>70</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1316,8 +2577,28 @@
       <c r="F10" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="Q10">
+        <f>Q9-SUM(M19:M21)</f>
+        <v>53</v>
+      </c>
+      <c r="R10">
+        <f>R9-SUM(N19:N21)</f>
+        <v>59</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1336,8 +2617,28 @@
       <c r="F11" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="Q11">
+        <f>Q10-SUM(M22:M24)</f>
+        <v>46</v>
+      </c>
+      <c r="R11">
+        <f>R10-SUM(N22:N24)</f>
+        <v>52</v>
+      </c>
+      <c r="S11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1356,8 +2657,28 @@
       <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="Q12">
+        <f>Q11-SUM(M25:M26)</f>
+        <v>41</v>
+      </c>
+      <c r="R12">
+        <f>R11-SUM(N25:N26)</f>
+        <v>46</v>
+      </c>
+      <c r="S12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1376,8 +2697,28 @@
       <c r="F13" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <f>Q12-SUM(M27:M29)</f>
+        <v>34</v>
+      </c>
+      <c r="R13">
+        <f>R12-SUM(N27:N29)</f>
+        <v>40</v>
+      </c>
+      <c r="S13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1396,8 +2737,28 @@
       <c r="F14" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <f>Q13-SUM(M30:M33)</f>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f>R13-SUM(N30:N33)</f>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1416,8 +2777,17 @@
       <c r="F15" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1436,8 +2806,17 @@
       <c r="F16" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1456,8 +2835,17 @@
       <c r="F17" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1476,8 +2864,17 @@
       <c r="F18" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1496,8 +2893,17 @@
       <c r="F19" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1516,8 +2922,17 @@
       <c r="F20" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1536,8 +2951,17 @@
       <c r="F21" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1556,8 +2980,17 @@
       <c r="F22" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1576,8 +3009,17 @@
       <c r="F23" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1596,13 +3038,22 @@
       <c r="F24" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1616,13 +3067,22 @@
       <c r="F25" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1636,8 +3096,17 @@
       <c r="F26" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>5</v>
+      </c>
+      <c r="O26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1648,7 +3117,7 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>54</v>
@@ -1656,8 +3125,17 @@
       <c r="F27" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1676,8 +3154,17 @@
       <c r="F28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1696,8 +3183,17 @@
       <c r="F29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>3</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1713,11 +3209,18 @@
       <c r="E30" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1733,11 +3236,18 @@
       <c r="E31" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1753,11 +3263,18 @@
       <c r="E32" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+      <c r="M32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1773,9 +3290,32 @@
       <c r="E33" t="s">
         <v>59</v>
       </c>
+      <c r="M33">
+        <v>25</v>
+      </c>
+      <c r="N33">
+        <v>30</v>
+      </c>
+      <c r="O33" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <f>SUM(M2:M33)</f>
+        <v>118</v>
+      </c>
+      <c r="N34">
+        <f>SUM(N2:N33)</f>
+        <v>129</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="M2:O33">
+    <sortCondition ref="O2:O33"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1783,8 +3323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2037159B-319A-4C42-A294-2B2489B57574}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,7 +3415,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1889,7 +3429,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1903,7 +3443,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1917,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1969,6 +3509,9 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
       <c r="E13" t="s">
         <v>50</v>
       </c>
@@ -1987,18 +3530,16 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2015,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2032,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2049,7 +3590,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2066,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2083,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2200,7 +3741,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
         <v>54</v>
@@ -2208,12 +3749,12 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
when group created the created is added and he cant remove himself from it
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="88">
   <si>
     <t>Play song</t>
   </si>
@@ -163,15 +163,9 @@
     <t>exceptions</t>
   </si>
   <si>
-    <t>tests</t>
-  </si>
-  <si>
     <t>burn down chart</t>
   </si>
   <si>
-    <t>db refactoring</t>
-  </si>
-  <si>
     <t>Stoicho</t>
   </si>
   <si>
@@ -181,12 +175,6 @@
     <t>Hannes</t>
   </si>
   <si>
-    <t>Each of us</t>
-  </si>
-  <si>
-    <t>Message encryption</t>
-  </si>
-  <si>
     <t>Ralfs</t>
   </si>
   <si>
@@ -247,9 +235,6 @@
     <t>Delete group</t>
   </si>
   <si>
-    <t>Updated person updated in all chats</t>
-  </si>
-  <si>
     <t>Remove notifications</t>
   </si>
   <si>
@@ -272,6 +257,36 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>Get playlist</t>
+  </si>
+  <si>
+    <t>One person can be logged in at once</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout </t>
+  </si>
+  <si>
+    <t>Multiplayer game</t>
+  </si>
+  <si>
+    <t>Game error</t>
+  </si>
+  <si>
+    <t>Report planing</t>
+  </si>
+  <si>
+    <t>Spreading tasks</t>
+  </si>
+  <si>
+    <t>All of us together</t>
+  </si>
+  <si>
+    <t>Updating end expanding existing UI</t>
+  </si>
+  <si>
+    <t>Not done</t>
   </si>
 </sst>
 </file>
@@ -405,11 +420,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$S$2:$S$14</c15:sqref>
+                    <c15:sqref>'Sprint 1'!$S$3:$S$15</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Sprint 1'!$S$2:$S$14</c:f>
+              <c:f>'Sprint 1'!$S$3:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -460,11 +475,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$Q$2:$Q$34</c15:sqref>
+                    <c15:sqref>'Sprint 1'!$Q$3:$Q$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Sprint 1'!$Q$2:$Q$14</c:f>
+              <c:f>'Sprint 1'!$Q$3:$Q$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -560,11 +575,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$S$2:$S$14</c15:sqref>
+                    <c15:sqref>'Sprint 1'!$S$3:$S$15</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Sprint 1'!$S$2:$S$14</c:f>
+              <c:f>'Sprint 1'!$S$3:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -615,11 +630,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$R$2:$R$34</c15:sqref>
+                    <c15:sqref>'Sprint 1'!$R$3:$R$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Sprint 1'!$R$2:$R$14</c:f>
+              <c:f>'Sprint 1'!$R$3:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -914,54 +929,50 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$S$2:$S$14</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$S$2:$S$14</c:f>
+              <c:f>'Sprint 1'!$S$2:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
@@ -969,54 +980,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$Q$2:$Q$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$Q$2:$Q$14</c:f>
+              <c:f>'Sprint 1'!$Q$2:$Q$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>101</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>68</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1069,54 +1076,50 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$S$2:$S$14</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$S$2:$S$14</c:f>
+              <c:f>'Sprint 1'!$S$2:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
@@ -1124,54 +1127,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$R$2:$R$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$R$2:$R$14</c:f>
+              <c:f>'Sprint 1'!$R$2:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>113</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>105</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>99</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>72</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1193,6 +1192,414 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="488277248"/>
+        <c:axId val="488277576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="488277248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="lv-LV"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488277576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488277576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="lv-LV"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488277248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="lv-LV"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="lv-LV"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.3803149606299209E-2"/>
+          <c:y val="3.7037037037037035E-2"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$M:$M</c:f>
+              <c:strCache>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>Estimate</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$O$2:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-26A2-4469-9AC6-DAD0A002A0F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$O$2:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$N$2:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-26A2-4469-9AC6-DAD0A002A0F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:smooth val="0"/>
         <c:axId val="488277248"/>
         <c:axId val="488277576"/>
@@ -1436,6 +1843,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2089,6 +2533,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2510,6 +3470,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>503465</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramma 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A75515-41B4-4775-954A-E404F04918DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2809,7 +3812,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -2824,13 +3827,13 @@
         <v>3</v>
       </c>
       <c r="Q1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="S1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="T1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2841,7 +3844,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -2878,7 +3881,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2915,7 +3918,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -2952,7 +3955,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2989,7 +3992,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -3026,7 +4029,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3063,7 +4066,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -3100,7 +4103,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -3137,7 +4140,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -3174,7 +4177,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -3211,7 +4214,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -3248,7 +4251,7 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -3285,7 +4288,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -3322,7 +4325,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -3351,7 +4354,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -3380,7 +4383,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -3409,7 +4412,7 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -3438,7 +4441,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -3467,7 +4470,7 @@
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3496,7 +4499,7 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -3525,7 +4528,7 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -3554,7 +4557,7 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -3583,7 +4586,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -3609,10 +4612,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -3638,10 +4641,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -3667,10 +4670,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -3699,7 +4702,7 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -3725,10 +4728,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D29">
         <v>6</v>
@@ -3754,10 +4757,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -3783,10 +4786,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -3812,10 +4815,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -3844,7 +4847,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D33">
         <v>25</v>
@@ -3934,7 +4937,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
         <v>42</v>
@@ -3948,7 +4951,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
         <v>42</v>
@@ -3962,7 +4965,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
@@ -3976,7 +4979,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
         <v>42</v>
@@ -3993,7 +4996,7 @@
         <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="U42">
         <v>41</v>
@@ -4007,7 +5010,7 @@
         <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -4037,7 +5040,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>42</v>
@@ -4048,7 +5051,7 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>42</v>
@@ -4059,7 +5062,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
         <v>42</v>
@@ -4070,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
@@ -4081,7 +5084,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
         <v>42</v>
@@ -4092,7 +5095,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
         <v>42</v>
@@ -4106,7 +5109,7 @@
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4128,7 +5131,7 @@
         <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4141,8 +5144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,13 +5182,13 @@
         <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="Q1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4202,7 +5205,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -4214,52 +5217,52 @@
         <v>1</v>
       </c>
       <c r="Q2">
+        <f>M34</f>
+        <v>118</v>
+      </c>
+      <c r="R2">
+        <f>N34</f>
+        <v>129</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <f>M34-SUM(M2:M5)</f>
         <v>104</v>
       </c>
-      <c r="R2">
+      <c r="R3">
         <f>N34-SUM(N2:N5)</f>
         <v>113</v>
       </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <f>Q2-SUM(M6)</f>
-        <v>101</v>
-      </c>
-      <c r="R3">
-        <f>R2-SUM(N6)</f>
-        <v>110</v>
-      </c>
       <c r="S3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -4276,7 +5279,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M4">
         <v>6</v>
@@ -4288,15 +5291,15 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <f>Q3-SUM(M7:M8)</f>
-        <v>97</v>
+        <f>Q3-SUM(M6)</f>
+        <v>101</v>
       </c>
       <c r="R4">
-        <f>R3-SUM(N7:N8)</f>
-        <v>105</v>
+        <f>R3-SUM(N6)</f>
+        <v>110</v>
       </c>
       <c r="S4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -4313,7 +5316,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -4325,15 +5328,15 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <f>Q4-SUM(M9:M10)</f>
-        <v>91</v>
+        <f>Q4-SUM(M7:M8)</f>
+        <v>97</v>
       </c>
       <c r="R5">
-        <f>R4-SUM(N9:N10)</f>
-        <v>99</v>
+        <f>R4-SUM(N7:N8)</f>
+        <v>105</v>
       </c>
       <c r="S5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -4350,7 +5353,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M6">
         <v>3</v>
@@ -4362,15 +5365,15 @@
         <v>2</v>
       </c>
       <c r="Q6">
-        <f>Q5-SUM(M11:M12)</f>
-        <v>86</v>
+        <f>Q5-SUM(M9:M10)</f>
+        <v>91</v>
       </c>
       <c r="R6">
-        <f>R5-SUM(N11:N12)</f>
-        <v>95</v>
+        <f>R5-SUM(N9:N10)</f>
+        <v>99</v>
       </c>
       <c r="S6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -4387,7 +5390,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M7">
         <v>2</v>
@@ -4399,15 +5402,15 @@
         <v>3</v>
       </c>
       <c r="Q7">
-        <f>Q6-SUM(M13:M15)</f>
-        <v>77</v>
+        <f>Q6-SUM(M11:M12)</f>
+        <v>86</v>
       </c>
       <c r="R7">
-        <f>R6-SUM(N13:N15)</f>
-        <v>86</v>
+        <f>R6-SUM(N11:N12)</f>
+        <v>95</v>
       </c>
       <c r="S7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4424,10 +5427,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M8">
         <v>2</v>
@@ -4439,15 +5442,15 @@
         <v>3</v>
       </c>
       <c r="Q8">
-        <f>Q7-SUM(M16:M17)</f>
-        <v>68</v>
+        <f>Q7-SUM(M13:M15)</f>
+        <v>77</v>
       </c>
       <c r="R8">
-        <f>R7-SUM(N16:N17)</f>
-        <v>72</v>
+        <f>R7-SUM(N13:N15)</f>
+        <v>86</v>
       </c>
       <c r="S8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -4464,10 +5467,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -4479,15 +5482,15 @@
         <v>4</v>
       </c>
       <c r="Q9">
-        <f>Q8-SUM(M18)</f>
-        <v>65</v>
+        <f>Q8-SUM(M16:M17)</f>
+        <v>68</v>
       </c>
       <c r="R9">
-        <f>R8-SUM(N18)</f>
-        <v>70</v>
+        <f>R8-SUM(N16:N17)</f>
+        <v>72</v>
       </c>
       <c r="S9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -4504,10 +5507,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M10">
         <v>4</v>
@@ -4519,15 +5522,15 @@
         <v>4</v>
       </c>
       <c r="Q10">
-        <f>Q9-SUM(M19:M21)</f>
-        <v>53</v>
+        <f>Q9-SUM(M18)</f>
+        <v>65</v>
       </c>
       <c r="R10">
-        <f>R9-SUM(N19:N21)</f>
-        <v>59</v>
+        <f>R9-SUM(N18)</f>
+        <v>70</v>
       </c>
       <c r="S10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -4544,10 +5547,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M11">
         <v>3</v>
@@ -4559,15 +5562,15 @@
         <v>5</v>
       </c>
       <c r="Q11">
-        <f>Q10-SUM(M22:M24)</f>
-        <v>46</v>
+        <f>Q10-SUM(M19:M21)</f>
+        <v>53</v>
       </c>
       <c r="R11">
-        <f>R10-SUM(N22:N24)</f>
-        <v>52</v>
+        <f>R10-SUM(N19:N21)</f>
+        <v>59</v>
       </c>
       <c r="S11">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -4584,10 +5587,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M12">
         <v>2</v>
@@ -4599,15 +5602,15 @@
         <v>5</v>
       </c>
       <c r="Q12">
-        <f>Q11-SUM(M25:M26)</f>
-        <v>41</v>
+        <f>Q11-SUM(M22:M24)</f>
+        <v>46</v>
       </c>
       <c r="R12">
-        <f>R11-SUM(N25:N26)</f>
-        <v>46</v>
+        <f>R11-SUM(N22:N24)</f>
+        <v>52</v>
       </c>
       <c r="S12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -4624,10 +5627,10 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M13">
         <v>4</v>
@@ -4639,15 +5642,15 @@
         <v>6</v>
       </c>
       <c r="Q13">
-        <f>Q12-SUM(M27:M29)</f>
-        <v>34</v>
+        <f>Q12-SUM(M25:M26)</f>
+        <v>41</v>
       </c>
       <c r="R13">
-        <f>R12-SUM(N27:N29)</f>
-        <v>40</v>
+        <f>R12-SUM(N25:N26)</f>
+        <v>46</v>
       </c>
       <c r="S13">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -4664,10 +5667,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -4679,15 +5682,15 @@
         <v>6</v>
       </c>
       <c r="Q14">
-        <f>Q13-SUM(M30:M33)</f>
-        <v>0</v>
+        <f>Q13-SUM(M27:M29)</f>
+        <v>34</v>
       </c>
       <c r="R14">
-        <f>R13-SUM(N30:N33)</f>
-        <v>0</v>
+        <f>R13-SUM(N27:N29)</f>
+        <v>40</v>
       </c>
       <c r="S14">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -4704,10 +5707,10 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M15">
         <v>2</v>
@@ -4718,6 +5721,17 @@
       <c r="O15">
         <v>6</v>
       </c>
+      <c r="Q15">
+        <f>Q14-SUM(M30:M33)</f>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f>R14-SUM(N30:N33)</f>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -4733,10 +5747,10 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M16">
         <v>6</v>
@@ -4762,10 +5776,10 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M17">
         <v>3</v>
@@ -4791,10 +5805,10 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M18">
         <v>3</v>
@@ -4820,10 +5834,10 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M19">
         <v>5</v>
@@ -4849,10 +5863,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M20">
         <v>4</v>
@@ -4878,10 +5892,10 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M21">
         <v>3</v>
@@ -4907,10 +5921,10 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M22">
         <v>2</v>
@@ -4936,10 +5950,10 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M23">
         <v>3</v>
@@ -4965,10 +5979,10 @@
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M24">
         <v>2</v>
@@ -4985,7 +5999,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -4994,10 +6008,10 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -5014,7 +6028,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -5023,10 +6037,10 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M26">
         <v>4</v>
@@ -5043,7 +6057,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -5052,10 +6066,10 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M27">
         <v>2</v>
@@ -5081,10 +6095,10 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M28">
         <v>2</v>
@@ -5101,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -5110,10 +6124,10 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M29">
         <v>3</v>
@@ -5130,7 +6144,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -5139,7 +6153,7 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F30" s="1"/>
       <c r="M30">
@@ -5157,7 +6171,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -5166,7 +6180,7 @@
         <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F31" s="1"/>
       <c r="M31">
@@ -5184,7 +6198,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -5193,7 +6207,7 @@
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F32" s="1"/>
       <c r="M32">
@@ -5220,7 +6234,7 @@
         <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M33">
         <v>25</v>
@@ -5253,20 +6267,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2037159B-319A-4C42-A294-2B2489B57574}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5285,8 +6300,23 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5296,11 +6326,37 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
       <c r="E2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <f>I26</f>
+        <v>81</v>
+      </c>
+      <c r="N2">
+        <f>J26</f>
+        <v>90</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5310,362 +6366,828 @@
       <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f>I26-SUM(I2:I5)</f>
+        <v>74</v>
+      </c>
+      <c r="N3">
+        <f>J26-SUM(J2:J5)</f>
+        <v>75</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f>M3-SUM(I6:I10)</f>
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="N4">
+        <f>N3-SUM(J6:J10)</f>
+        <v>45</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f>M4-SUM(I11:I14)</f>
+        <v>32</v>
+      </c>
+      <c r="N5">
+        <f>N4-SUM(J11:J14)</f>
+        <v>28</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <f>M5-SUM(I15:I17)</f>
+        <v>26</v>
+      </c>
+      <c r="N6">
+        <f>N5-SUM(J15:J17)</f>
+        <v>20</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <f>M6-SUM(I18:I23)</f>
+        <v>11</v>
+      </c>
+      <c r="N7">
+        <f>N6-SUM(J18:J23)</f>
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f>M7-SUM(I24:I25)</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>N7-SUM(J24:J25)</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>24</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10">
+      <c r="F22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="K24">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
         <v>45</v>
       </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <f>SUM(I2:I25)</f>
+        <v>81</v>
+      </c>
+      <c r="J26">
+        <f>SUM(J2:J25)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28">
         <v>8</v>
       </c>
-      <c r="E22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" t="s">
-        <v>54</v>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Database fixed for- Group,Chat and message; Chat and message refresh the onnection (should not be eny exceptions)
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="93">
   <si>
     <t>Play song</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Reports</t>
   </si>
   <si>
-    <t>transactions isolaton</t>
-  </si>
-  <si>
     <t>Stoycho</t>
   </si>
   <si>
@@ -299,6 +296,12 @@
   </si>
   <si>
     <t>Splitting report tasks</t>
+  </si>
+  <si>
+    <t>Fix update profile</t>
+  </si>
+  <si>
+    <t>transactions</t>
   </si>
 </sst>
 </file>
@@ -6256,7 +6259,7 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>
@@ -6289,7 +6292,7 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" t="s">
         <v>44</v>
@@ -6522,7 +6525,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -6563,7 +6566,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -6604,7 +6607,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -6645,7 +6648,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -6686,7 +6689,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -6731,7 +6734,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -7347,7 +7350,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24">
@@ -7511,10 +7514,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7884E-D22C-4C15-B48F-DDAEB03C83F5}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7574,7 +7577,7 @@
         <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>43</v>
@@ -7604,10 +7607,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
         <v>89</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7615,7 +7618,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
@@ -7624,14 +7627,40 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>87</v>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mvc updates password is hidden and chats are displayed differently
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -8,10 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint 3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint 0" sheetId="6" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId5"/>
+    <sheet name="Sprint 4" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="114">
   <si>
     <t>Play song</t>
   </si>
@@ -302,6 +303,69 @@
   </si>
   <si>
     <t>transactions</t>
+  </si>
+  <si>
+    <t>Mock up</t>
+  </si>
+  <si>
+    <t>MoSCoW</t>
+  </si>
+  <si>
+    <t>Use cases</t>
+  </si>
+  <si>
+    <t>Group Contract</t>
+  </si>
+  <si>
+    <t>Domain model</t>
+  </si>
+  <si>
+    <t>Database model</t>
+  </si>
+  <si>
+    <t>Drop database script</t>
+  </si>
+  <si>
+    <t>Database table creation scripts</t>
+  </si>
+  <si>
+    <t>Database insert row scripts scripts</t>
+  </si>
+  <si>
+    <t>Domain model explanation</t>
+  </si>
+  <si>
+    <t>Distribute usecases</t>
+  </si>
+  <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>User stories</t>
+  </si>
+  <si>
+    <t>Create report structure</t>
+  </si>
+  <si>
+    <t>Database triger tests</t>
+  </si>
+  <si>
+    <t>Read about chats</t>
+  </si>
+  <si>
+    <t>Decide on development method</t>
+  </si>
+  <si>
+    <t>Establish coding standards</t>
+  </si>
+  <si>
+    <t>Agree on working conditions</t>
+  </si>
+  <si>
+    <t>Generate product idea</t>
+  </si>
+  <si>
+    <t>Do it!</t>
   </si>
 </sst>
 </file>
@@ -408,7 +472,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1'!$Q$1</c:f>
+              <c:f>'Sprint 0'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -443,109 +507,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$S$3:$S$15</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$S$3:$S$15</c:f>
+              <c:f>'Sprint 0'!$O$2:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$Q$3:$Q$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$Q$3:$Q$15</c:f>
+              <c:f>'Sprint 0'!$M$2:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -554,7 +562,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7E1A-443C-8892-BDFC65A0A0A1}"/>
+              <c16:uniqueId val="{00000002-A33C-438A-9A29-801E903EE326}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -563,7 +571,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1'!$R$1</c:f>
+              <c:f>'Sprint 0'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -598,109 +606,53 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$S$3:$S$15</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$S$3:$S$15</c:f>
+              <c:f>'Sprint 0'!$O$2:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Sprint 1'!$R$3:$R$34</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Sprint 1'!$R$3:$R$15</c:f>
+              <c:f>'Sprint 0'!$N$2:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>113</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>105</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -709,7 +661,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7E1A-443C-8892-BDFC65A0A0A1}"/>
+              <c16:uniqueId val="{00000003-A33C-438A-9A29-801E903EE326}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1412,122 +1364,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sprint 2'!$M:$M</c:f>
-              <c:strCache>
-                <c:ptCount val="1048576"/>
-                <c:pt idx="0">
-                  <c:v>Estimate</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sprint 2'!$O$2:$O$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 2'!$M$2:$M$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-26A2-4469-9AC6-DAD0A002A0F5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Sprint 2'!$N$1</c:f>
@@ -1542,14 +1380,26 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1618,6 +1468,81 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F94-48BA-8251-850259E5A8DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1626,6 +1551,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="488277248"/>
         <c:axId val="488277576"/>
@@ -1870,10 +1796,13 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -2913,7 +2842,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3021,11 +2950,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3036,11 +2960,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3072,9 +2991,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3432,23 +3348,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>299358</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>131989</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>312964</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>13606</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>17689</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramma 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA8B0D07-D641-49D4-91D0-7D9753D97F44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A90F5E9A-3702-4EF0-A1FC-776B1F2DDFED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3818,10 +3734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A58" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W72" sqref="W72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3830,7 +3746,7 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -3846,23 +3762,8 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3878,28 +3779,8 @@
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="O2">
-        <v>3</v>
-      </c>
-      <c r="P2">
-        <v>5</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <f>O34-SUM(O2:O5)</f>
-        <v>104</v>
-      </c>
-      <c r="T2">
-        <f>P34-SUM(P2:P5)</f>
-        <v>113</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3915,28 +3796,8 @@
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="O3">
-        <v>3</v>
-      </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <f>S2-SUM(O6)</f>
-        <v>101</v>
-      </c>
-      <c r="T3">
-        <f>T2-SUM(P6)</f>
-        <v>110</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3952,28 +3813,8 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="O4">
-        <v>6</v>
-      </c>
-      <c r="P4">
-        <v>6</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <f>S3-SUM(O7:O8)</f>
-        <v>97</v>
-      </c>
-      <c r="T4">
-        <f>T3-SUM(P7:P8)</f>
-        <v>105</v>
-      </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3989,28 +3830,8 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
-        <v>2</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <f>S4-SUM(O9:O10)</f>
-        <v>91</v>
-      </c>
-      <c r="T5">
-        <f>T4-SUM(P9:P10)</f>
-        <v>99</v>
-      </c>
-      <c r="U5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4026,28 +3847,8 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6">
-        <v>3</v>
-      </c>
-      <c r="Q6">
-        <v>2</v>
-      </c>
-      <c r="S6">
-        <f>S5-SUM(O11:O12)</f>
-        <v>86</v>
-      </c>
-      <c r="T6">
-        <f>T5-SUM(P11:P12)</f>
-        <v>95</v>
-      </c>
-      <c r="U6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4063,28 +3864,8 @@
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
-      <c r="P7">
-        <v>3</v>
-      </c>
-      <c r="Q7">
-        <v>3</v>
-      </c>
-      <c r="S7">
-        <f>S6-SUM(O13:O15)</f>
-        <v>77</v>
-      </c>
-      <c r="T7">
-        <f>T6-SUM(P13:P15)</f>
-        <v>86</v>
-      </c>
-      <c r="U7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4100,28 +3881,8 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="O8">
-        <v>2</v>
-      </c>
-      <c r="P8">
-        <v>2</v>
-      </c>
-      <c r="Q8">
-        <v>3</v>
-      </c>
-      <c r="S8">
-        <f>S7-SUM(O16:O17)</f>
-        <v>68</v>
-      </c>
-      <c r="T8">
-        <f>T7-SUM(P16:P17)</f>
-        <v>72</v>
-      </c>
-      <c r="U8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4137,28 +3898,8 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="O9">
-        <v>2</v>
-      </c>
-      <c r="P9">
-        <v>2</v>
-      </c>
-      <c r="Q9">
-        <v>4</v>
-      </c>
-      <c r="S9">
-        <f>S8-SUM(O18)</f>
-        <v>65</v>
-      </c>
-      <c r="T9">
-        <f>T8-SUM(P18)</f>
-        <v>70</v>
-      </c>
-      <c r="U9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4174,28 +3915,8 @@
       <c r="E10">
         <v>3</v>
       </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <v>4</v>
-      </c>
-      <c r="Q10">
-        <v>4</v>
-      </c>
-      <c r="S10">
-        <f>S9-SUM(O19:O21)</f>
-        <v>53</v>
-      </c>
-      <c r="T10">
-        <f>T9-SUM(P19:P21)</f>
-        <v>59</v>
-      </c>
-      <c r="U10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4211,28 +3932,8 @@
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="O11">
-        <v>3</v>
-      </c>
-      <c r="P11">
-        <v>3</v>
-      </c>
-      <c r="Q11">
-        <v>5</v>
-      </c>
-      <c r="S11">
-        <f>S10-SUM(O22:O24)</f>
-        <v>46</v>
-      </c>
-      <c r="T11">
-        <f>T10-SUM(P22:P24)</f>
-        <v>52</v>
-      </c>
-      <c r="U11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4248,28 +3949,8 @@
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="O12">
-        <v>2</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>5</v>
-      </c>
-      <c r="S12">
-        <f>S11-SUM(O25:O26)</f>
-        <v>41</v>
-      </c>
-      <c r="T12">
-        <f>T11-SUM(P25:P26)</f>
-        <v>46</v>
-      </c>
-      <c r="U12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4285,28 +3966,8 @@
       <c r="E13">
         <v>4</v>
       </c>
-      <c r="O13">
-        <v>4</v>
-      </c>
-      <c r="P13">
-        <v>4</v>
-      </c>
-      <c r="Q13">
-        <v>6</v>
-      </c>
-      <c r="S13">
-        <f>S12-SUM(O27:O29)</f>
-        <v>34</v>
-      </c>
-      <c r="T13">
-        <f>T12-SUM(P27:P29)</f>
-        <v>40</v>
-      </c>
-      <c r="U13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -4322,28 +3983,8 @@
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="O14">
-        <v>3</v>
-      </c>
-      <c r="P14">
-        <v>3</v>
-      </c>
-      <c r="Q14">
-        <v>6</v>
-      </c>
-      <c r="S14">
-        <f>S13-SUM(O30:O33)</f>
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <f>T13-SUM(P30:P33)</f>
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -4359,20 +4000,8 @@
       <c r="E15">
         <v>4</v>
       </c>
-      <c r="O15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <v>2</v>
-      </c>
-      <c r="Q15">
-        <v>6</v>
-      </c>
-      <c r="U15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -4388,20 +4017,8 @@
       <c r="E16">
         <v>4</v>
       </c>
-      <c r="O16">
-        <v>6</v>
-      </c>
-      <c r="P16">
-        <v>10</v>
-      </c>
-      <c r="Q16">
-        <v>7</v>
-      </c>
-      <c r="U16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -4417,20 +4034,8 @@
       <c r="E17">
         <v>3</v>
       </c>
-      <c r="O17">
-        <v>3</v>
-      </c>
-      <c r="P17">
-        <v>4</v>
-      </c>
-      <c r="Q17">
-        <v>7</v>
-      </c>
-      <c r="U17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4446,20 +4051,8 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="O18">
-        <v>3</v>
-      </c>
-      <c r="P18">
-        <v>2</v>
-      </c>
-      <c r="Q18">
-        <v>8</v>
-      </c>
-      <c r="U18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -4475,20 +4068,8 @@
       <c r="E19">
         <v>3</v>
       </c>
-      <c r="O19">
-        <v>5</v>
-      </c>
-      <c r="P19">
-        <v>4</v>
-      </c>
-      <c r="Q19">
-        <v>9</v>
-      </c>
-      <c r="U19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4504,20 +4085,8 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="O20">
-        <v>4</v>
-      </c>
-      <c r="P20">
-        <v>4</v>
-      </c>
-      <c r="Q20">
-        <v>9</v>
-      </c>
-      <c r="U20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4533,20 +4102,8 @@
       <c r="E21">
         <v>2</v>
       </c>
-      <c r="O21">
-        <v>3</v>
-      </c>
-      <c r="P21">
-        <v>3</v>
-      </c>
-      <c r="Q21">
-        <v>9</v>
-      </c>
-      <c r="U21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -4562,20 +4119,8 @@
       <c r="E22">
         <v>2</v>
       </c>
-      <c r="O22">
-        <v>2</v>
-      </c>
-      <c r="P22">
-        <v>2</v>
-      </c>
-      <c r="Q22">
-        <v>10</v>
-      </c>
-      <c r="U22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4591,20 +4136,8 @@
       <c r="E23">
         <v>2</v>
       </c>
-      <c r="O23">
-        <v>3</v>
-      </c>
-      <c r="P23">
-        <v>2</v>
-      </c>
-      <c r="Q23">
-        <v>10</v>
-      </c>
-      <c r="U23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -4620,20 +4153,8 @@
       <c r="E24">
         <v>4</v>
       </c>
-      <c r="O24">
-        <v>2</v>
-      </c>
-      <c r="P24">
-        <v>3</v>
-      </c>
-      <c r="Q24">
-        <v>10</v>
-      </c>
-      <c r="U24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -4649,20 +4170,8 @@
       <c r="E25">
         <v>4</v>
       </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>11</v>
-      </c>
-      <c r="U25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4678,20 +4187,8 @@
       <c r="E26">
         <v>2</v>
       </c>
-      <c r="O26">
-        <v>4</v>
-      </c>
-      <c r="P26">
-        <v>5</v>
-      </c>
-      <c r="Q26">
-        <v>11</v>
-      </c>
-      <c r="U26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -4707,20 +4204,8 @@
       <c r="E27">
         <v>10</v>
       </c>
-      <c r="O27">
-        <v>2</v>
-      </c>
-      <c r="P27">
-        <v>2</v>
-      </c>
-      <c r="Q27">
-        <v>12</v>
-      </c>
-      <c r="U27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -4736,20 +4221,8 @@
       <c r="E28">
         <v>5</v>
       </c>
-      <c r="O28">
-        <v>2</v>
-      </c>
-      <c r="P28">
-        <v>2</v>
-      </c>
-      <c r="Q28">
-        <v>12</v>
-      </c>
-      <c r="U28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4765,20 +4238,8 @@
       <c r="E29">
         <v>6</v>
       </c>
-      <c r="O29">
-        <v>3</v>
-      </c>
-      <c r="P29">
-        <v>2</v>
-      </c>
-      <c r="Q29">
-        <v>12</v>
-      </c>
-      <c r="U29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -4794,20 +4255,8 @@
       <c r="E30">
         <v>2</v>
       </c>
-      <c r="O30">
-        <v>4</v>
-      </c>
-      <c r="P30">
-        <v>4</v>
-      </c>
-      <c r="Q30">
-        <v>13</v>
-      </c>
-      <c r="U30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4823,20 +4272,8 @@
       <c r="E31">
         <v>4</v>
       </c>
-      <c r="O31">
-        <v>3</v>
-      </c>
-      <c r="P31">
-        <v>4</v>
-      </c>
-      <c r="Q31">
-        <v>13</v>
-      </c>
-      <c r="U31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -4852,20 +4289,8 @@
       <c r="E32">
         <v>4</v>
       </c>
-      <c r="O32">
-        <v>2</v>
-      </c>
-      <c r="P32">
-        <v>2</v>
-      </c>
-      <c r="Q32">
-        <v>13</v>
-      </c>
-      <c r="U32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4881,20 +4306,9 @@
       <c r="E33">
         <v>30</v>
       </c>
-      <c r="O33">
-        <v>25</v>
-      </c>
-      <c r="P33">
-        <v>30</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>13</v>
-      </c>
-      <c r="U33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4910,19 +4324,8 @@
       <c r="E34">
         <v>2</v>
       </c>
-      <c r="O34">
-        <f>SUM(O2:O33)</f>
-        <v>118</v>
-      </c>
-      <c r="P34">
-        <f>SUM(P2:P33)</f>
-        <v>129</v>
-      </c>
-      <c r="U34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4938,11 +4341,8 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="U35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -4958,11 +4358,8 @@
       <c r="E36">
         <v>3</v>
       </c>
-      <c r="U36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -4978,11 +4375,8 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="U37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -4998,11 +4392,8 @@
       <c r="E38">
         <v>2</v>
       </c>
-      <c r="U38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -5018,11 +4409,8 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="U39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -5038,11 +4426,8 @@
       <c r="E40">
         <v>5</v>
       </c>
-      <c r="U40">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -5058,11 +4443,8 @@
       <c r="E41">
         <v>2</v>
       </c>
-      <c r="U41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -5078,11 +4460,8 @@
       <c r="E42">
         <v>2</v>
       </c>
-      <c r="U42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -5099,7 +4478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -5116,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -5133,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -5150,7 +4529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -5167,7 +4546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -5203,13 +4582,19 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>66</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -5217,10 +4602,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>66</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -5228,10 +4619,1018 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62">
+        <v>7</v>
+      </c>
+      <c r="E62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65">
+        <v>10</v>
+      </c>
+      <c r="E65">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C69" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
         <v>84</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C72" t="s">
         <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416D8BE7-F174-4DE6-8BD7-669440759E00}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <f>I22</f>
+        <v>88</v>
+      </c>
+      <c r="N2" s="3">
+        <f>J22</f>
+        <v>96</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <f>M2-SUM(I2:I3)</f>
+        <v>69</v>
+      </c>
+      <c r="N3" s="3">
+        <f>N2-SUM(J2:J3)</f>
+        <v>73</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3">
+        <f>M3-SUM(I4:I8)</f>
+        <v>45</v>
+      </c>
+      <c r="N4" s="3">
+        <f>N3-SUM(J4:J8)</f>
+        <v>50</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f>M4-SUM(I9:I12)</f>
+        <v>25</v>
+      </c>
+      <c r="N5" s="3">
+        <f>N4-SUM(J9:J12)</f>
+        <v>27</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <f>M5-SUM(I13:I17)</f>
+        <v>16</v>
+      </c>
+      <c r="N6" s="3">
+        <f>N5-SUM(J13:J17)</f>
+        <v>17</v>
+      </c>
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <f>M6-SUM(I18:I21)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <f>N6-SUM(J18:J21)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12">
+        <v>12</v>
+      </c>
+      <c r="J12">
+        <v>13</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <v>8</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f>SUM(I2:I21)</f>
+        <v>88</v>
+      </c>
+      <c r="J22">
+        <f>SUM(J2:J21)</f>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -5240,17 +5639,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -6458,12 +6857,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2037159B-319A-4C42-A294-2B2489B57574}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6527,9 +6926,6 @@
       <c r="E2" t="s">
         <v>87</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
@@ -6568,9 +6964,6 @@
       <c r="E3" t="s">
         <v>87</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
       <c r="I3" s="3">
         <v>2</v>
       </c>
@@ -6609,9 +7002,6 @@
       <c r="E4" t="s">
         <v>87</v>
       </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
       <c r="I4" s="3">
         <v>1</v>
       </c>
@@ -6650,9 +7040,6 @@
       <c r="E5" t="s">
         <v>87</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
       <c r="I5" s="3">
         <v>3</v>
       </c>
@@ -6691,13 +7078,6 @@
       <c r="E6" t="s">
         <v>87</v>
       </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <f>-H7</f>
-        <v>0</v>
-      </c>
       <c r="I6" s="3">
         <v>1</v>
       </c>
@@ -6736,12 +7116,6 @@
       <c r="E7" t="s">
         <v>87</v>
       </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
@@ -6783,9 +7157,6 @@
       <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
       <c r="I8" s="3">
         <v>2</v>
       </c>
@@ -6827,9 +7198,6 @@
       <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
       <c r="I9" s="3">
         <v>1</v>
       </c>
@@ -6863,9 +7231,6 @@
       <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="I10" s="3">
         <v>20</v>
       </c>
@@ -6899,9 +7264,6 @@
       <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
       <c r="I11" s="3">
         <v>8</v>
       </c>
@@ -6935,9 +7297,6 @@
       <c r="F12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
       <c r="I12" s="3">
         <v>2</v>
       </c>
@@ -6969,9 +7328,6 @@
         <v>41</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13">
-        <v>4</v>
-      </c>
       <c r="I13" s="3">
         <v>6</v>
       </c>
@@ -7002,9 +7358,6 @@
       <c r="E14" t="s">
         <v>41</v>
       </c>
-      <c r="G14">
-        <v>6</v>
-      </c>
       <c r="I14" s="3">
         <v>1</v>
       </c>
@@ -7035,9 +7388,6 @@
       <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="G15">
-        <v>6</v>
-      </c>
       <c r="I15" s="3">
         <v>1</v>
       </c>
@@ -7071,9 +7421,6 @@
       <c r="F16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
       <c r="I16" s="3">
         <v>4</v>
       </c>
@@ -7107,9 +7454,6 @@
       <c r="F17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
       <c r="I17" s="3">
         <v>1</v>
       </c>
@@ -7143,9 +7487,6 @@
       <c r="F18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
       <c r="I18" s="3">
         <v>1</v>
       </c>
@@ -7179,9 +7520,6 @@
       <c r="F19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
       <c r="I19" s="3">
         <v>1</v>
       </c>
@@ -7215,9 +7553,6 @@
       <c r="F20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
       <c r="I20" s="3">
         <v>5</v>
       </c>
@@ -7251,9 +7586,6 @@
       <c r="F21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
       <c r="I21" s="3">
         <v>4</v>
       </c>
@@ -7285,9 +7617,6 @@
         <v>39</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22">
-        <v>4</v>
-      </c>
       <c r="I22" s="3">
         <v>2</v>
       </c>
@@ -7319,9 +7648,6 @@
         <v>41</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23">
-        <v>5</v>
-      </c>
       <c r="I23" s="3">
         <v>2</v>
       </c>
@@ -7353,9 +7679,6 @@
         <v>87</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24">
-        <v>5</v>
-      </c>
       <c r="I24" s="3">
         <v>2</v>
       </c>
@@ -7385,9 +7708,6 @@
       <c r="E25" t="s">
         <v>40</v>
       </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
       <c r="I25" s="3">
         <v>1</v>
       </c>
@@ -7397,6 +7717,7 @@
       <c r="K25" s="3">
         <v>6</v>
       </c>
+      <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -7416,9 +7737,6 @@
       </c>
       <c r="E26" t="s">
         <v>74</v>
-      </c>
-      <c r="G26">
-        <v>5</v>
       </c>
       <c r="I26" s="3">
         <v>10</v>
@@ -7450,9 +7768,6 @@
       <c r="E27" t="s">
         <v>74</v>
       </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
       <c r="I27" s="3">
         <v>1</v>
       </c>
@@ -7479,9 +7794,6 @@
       </c>
       <c r="E28" t="s">
         <v>41</v>
-      </c>
-      <c r="G28">
-        <v>6</v>
       </c>
       <c r="I28" s="3">
         <v>1</v>
@@ -7512,11 +7824,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7884E-D22C-4C15-B48F-DDAEB03C83F5}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -7668,7 +7980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3C4868-DA68-4B79-A75F-C29998123D8F}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
updates to documentation(newesst sprint part, moscow, backlog and system dev. report plan)
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="137">
   <si>
     <t>Play song</t>
   </si>
@@ -245,54 +245,30 @@
     <t>Updating end expanding existing UI</t>
   </si>
   <si>
-    <t>MVC</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>WCF hosting</t>
   </si>
   <si>
     <t>Dos/Ddos protection</t>
   </si>
   <si>
-    <t>test/refactor code</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
-    <t>Entity framework</t>
-  </si>
-  <si>
     <t>Sys dev report</t>
   </si>
   <si>
     <t>Techno/Programming report</t>
   </si>
   <si>
-    <t>Reports</t>
-  </si>
-  <si>
     <t>Stoycho</t>
   </si>
   <si>
-    <t>Ajax spike</t>
-  </si>
-  <si>
-    <t>Andrei/Ralfs</t>
-  </si>
-  <si>
     <t>Splitting report tasks</t>
   </si>
   <si>
     <t>Fix update profile</t>
   </si>
   <si>
-    <t>transactions</t>
-  </si>
-  <si>
     <t>Mock up</t>
   </si>
   <si>
@@ -366,6 +342,99 @@
   </si>
   <si>
     <t>Chat users updated if user info changed</t>
+  </si>
+  <si>
+    <t>Signlr spike</t>
+  </si>
+  <si>
+    <t>MVC spike</t>
+  </si>
+  <si>
+    <t>Optimize transactions</t>
+  </si>
+  <si>
+    <t>Spike on WCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spike on different communication protocols </t>
+  </si>
+  <si>
+    <t>Spike on email sending</t>
+  </si>
+  <si>
+    <t>Sprint summup</t>
+  </si>
+  <si>
+    <t>Fix music player</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Plan driven Vs. Agile Development</t>
+  </si>
+  <si>
+    <t>Quality Criteria and Architecture</t>
+  </si>
+  <si>
+    <t>Development Method of Choice</t>
+  </si>
+  <si>
+    <t>merging Report</t>
+  </si>
+  <si>
+    <t>Giving feedback on report</t>
+  </si>
+  <si>
+    <t>Requesting edits for report</t>
+  </si>
+  <si>
+    <t>Final touches for report</t>
+  </si>
+  <si>
+    <t>Preliminary Study</t>
+  </si>
+  <si>
+    <t>Service’s Architecture</t>
+  </si>
+  <si>
+    <t>Database Architecture</t>
+  </si>
+  <si>
+    <t>Dedicated Client explanation</t>
+  </si>
+  <si>
+    <t>Web Client explanation</t>
+  </si>
+  <si>
+    <t>Choice of middleware</t>
+  </si>
+  <si>
+    <t>Security in program</t>
+  </si>
+  <si>
+    <t>Concurrency in project</t>
+  </si>
+  <si>
+    <t>Performance of project</t>
+  </si>
+  <si>
+    <t>Interesting bits of code</t>
+  </si>
+  <si>
+    <t>Epilogue</t>
+  </si>
+  <si>
+    <t>test/optimize code</t>
+  </si>
+  <si>
+    <t>MVC application</t>
+  </si>
+  <si>
+    <t>Quality Assurance</t>
+  </si>
+  <si>
+    <t>Types of Services</t>
   </si>
 </sst>
 </file>
@@ -408,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -418,6 +487,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -999,7 +1072,7 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1146,7 +1219,7 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1438,22 +1511,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>94</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1513,22 +1586,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1540,6 +1613,349 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3F94-48BA-8251-850259E5A8DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="488277248"/>
+        <c:axId val="488277576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="488277248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="lv-LV"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488277576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488277576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="lv-LV"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488277248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="lv-LV"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="lv-LV"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="lv-LV"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.3803149606299209E-2"/>
+          <c:y val="3.7037037037037035E-2"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 3'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 3'!$P$2:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$N$2:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AA41-45F6-B695-FBBBE507A130}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1835,6 +2251,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2842,6 +3298,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3449,6 +4408,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A75515-41B4-4775-954A-E404F04918DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>71238</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramma 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF380613-FA7D-48FD-B91D-BB9E3FBD5B40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3736,8 +4738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W72" sqref="W72"/>
+    <sheetView topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4585,7 +5587,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
         <v>64</v>
@@ -4602,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
         <v>64</v>
@@ -4619,7 +5621,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C52" t="s">
         <v>64</v>
@@ -4636,7 +5638,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
         <v>64</v>
@@ -4653,7 +5655,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
         <v>64</v>
@@ -4670,7 +5672,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C55" t="s">
         <v>64</v>
@@ -4687,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C56" t="s">
         <v>64</v>
@@ -4704,7 +5706,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
         <v>64</v>
@@ -4721,7 +5723,7 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
         <v>64</v>
@@ -4738,7 +5740,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
         <v>64</v>
@@ -4755,7 +5757,7 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
@@ -4772,7 +5774,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
         <v>64</v>
@@ -4789,7 +5791,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
         <v>64</v>
@@ -4806,7 +5808,7 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
         <v>64</v>
@@ -4823,7 +5825,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C64" t="s">
         <v>64</v>
@@ -4840,7 +5842,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C65" t="s">
         <v>64</v>
@@ -4857,7 +5859,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C66" t="s">
         <v>64</v>
@@ -4874,7 +5876,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C67" t="s">
         <v>64</v>
@@ -4891,7 +5893,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C68" t="s">
         <v>64</v>
@@ -4908,7 +5910,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
         <v>64</v>
@@ -4928,7 +5930,7 @@
         <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -4936,10 +5938,10 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4947,10 +5949,10 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -5015,7 +6017,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -5055,7 +6057,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -5095,7 +6097,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -5135,7 +6137,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5175,7 +6177,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -5212,7 +6214,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -5249,7 +6251,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -5258,7 +6260,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -5278,7 +6280,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -5304,7 +6306,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -5330,7 +6332,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5356,7 +6358,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -5382,7 +6384,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -5408,7 +6410,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -5434,7 +6436,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -5449,7 +6451,7 @@
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -5466,7 +6468,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -5495,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -5521,7 +6523,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -5550,7 +6552,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -5576,7 +6578,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -5602,7 +6604,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -5643,13 +6645,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="C3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -5922,23 +6924,21 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="M8" s="3">
         <v>2</v>
       </c>
@@ -5966,13 +6966,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -6007,7 +7007,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -6048,13 +7048,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -6089,7 +7089,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -6130,13 +7130,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -6171,13 +7171,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -6196,12 +7196,12 @@
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3">
-        <f>Q13-SUM(M27:M29)</f>
-        <v>34</v>
+        <f>Q13-SUM(M27:M31)</f>
+        <v>27</v>
       </c>
       <c r="R14" s="3">
-        <f>R13-SUM(N27:N29)</f>
-        <v>40</v>
+        <f>R13-SUM(N27:N31)</f>
+        <v>32</v>
       </c>
       <c r="S14" s="3">
         <v>12</v>
@@ -6212,13 +7212,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
@@ -6237,11 +7237,11 @@
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3">
-        <f>Q14-SUM(M30:M33)</f>
+        <f>Q14-SUM(M32:M33)</f>
         <v>0</v>
       </c>
       <c r="R15" s="3">
-        <f>R14-SUM(N30:N33)</f>
+        <f>R14-SUM(N32:N33)</f>
         <v>0</v>
       </c>
       <c r="S15" s="3">
@@ -6253,10 +7253,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -6286,13 +7286,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -6316,16 +7316,16 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -6349,16 +7349,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -6382,16 +7382,16 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
@@ -6415,16 +7415,16 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
@@ -6451,7 +7451,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -6481,13 +7481,13 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -6658,7 +7658,7 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
         <v>42</v>
@@ -6691,7 +7691,7 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
         <v>42</v>
@@ -6734,7 +7734,7 @@
         <v>4</v>
       </c>
       <c r="O30" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
@@ -6765,7 +7765,7 @@
         <v>4</v>
       </c>
       <c r="O31" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
@@ -6859,10 +7859,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2037159B-319A-4C42-A294-2B2489B57574}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6924,7 +7924,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -6937,12 +7937,12 @@
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3">
-        <f>I29</f>
-        <v>85</v>
+        <f>I32</f>
+        <v>91</v>
       </c>
       <c r="N2" s="3">
-        <f>J29</f>
-        <v>94</v>
+        <f>J32</f>
+        <v>99</v>
       </c>
       <c r="O2" s="3">
         <v>0</v>
@@ -6962,7 +7962,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -6975,12 +7975,12 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3">
-        <f>I29-SUM(I2:I5)</f>
-        <v>78</v>
+        <f>I32-SUM(I2:I5)</f>
+        <v>84</v>
       </c>
       <c r="N3" s="3">
-        <f>J29-SUM(J2:J5)</f>
-        <v>79</v>
+        <f>J32-SUM(J2:J5)</f>
+        <v>84</v>
       </c>
       <c r="O3" s="3">
         <v>1</v>
@@ -7000,7 +8000,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -7014,11 +8014,11 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3">
         <f>M3-SUM(I6:I10)</f>
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N4" s="3">
         <f>N3-SUM(J6:J10)</f>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="O4" s="3">
         <v>2</v>
@@ -7038,7 +8038,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
@@ -7052,11 +8052,11 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3">
         <f>M4-SUM(I11:I14)</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="N5" s="3">
         <f>N4-SUM(J11:J14)</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="O5" s="3">
         <v>3</v>
@@ -7076,7 +8076,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -7090,11 +8090,11 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3">
         <f>M5-SUM(I15:I17)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N6" s="3">
         <f>N5-SUM(J15:J17)</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="O6" s="3">
         <v>4</v>
@@ -7114,7 +8114,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
@@ -7128,11 +8128,11 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3">
         <f>M6-SUM(I18:I24)</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N7" s="3">
         <f>N6-SUM(J18:J24)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="O7" s="3">
         <v>5</v>
@@ -7168,11 +8168,11 @@
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3">
-        <f>M7-SUM(I25:I28)</f>
+        <f>M7-SUM(I25:I31)</f>
         <v>0</v>
       </c>
       <c r="N8" s="3">
-        <f>N7-SUM(J25:J28)</f>
+        <f>N7-SUM(J25:J31)</f>
         <v>0</v>
       </c>
       <c r="O8" s="3">
@@ -7184,7 +8184,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -7283,7 +8283,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -7605,7 +8605,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -7636,7 +8636,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -7667,7 +8667,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -7676,14 +8676,14 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F24" s="1"/>
       <c r="I24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" s="3">
         <v>5</v>
@@ -7697,7 +8697,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -7709,10 +8709,10 @@
         <v>39</v>
       </c>
       <c r="I25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="3">
         <v>6</v>
@@ -7739,10 +8739,10 @@
         <v>71</v>
       </c>
       <c r="I26" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J26" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K26" s="3">
         <v>6</v>
@@ -7769,10 +8769,10 @@
         <v>71</v>
       </c>
       <c r="I27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27" s="3">
         <v>6</v>
@@ -7784,7 +8784,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -7807,15 +8807,93 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
       <c r="I29" s="3">
-        <f>SUM(C2:C28)</f>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J29" s="3">
-        <f>SUM(D2:D28)</f>
-        <v>94</v>
-      </c>
-      <c r="K29" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="K29" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="3">
+        <f>SUM(C2:C31)</f>
+        <v>91</v>
+      </c>
+      <c r="J32" s="3">
+        <f>SUM(D2:D31)</f>
+        <v>99</v>
+      </c>
+      <c r="K32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7826,20 +8904,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7884E-D22C-4C15-B48F-DDAEB03C83F5}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7858,138 +8936,832 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>73</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
       <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <f>I31</f>
+        <v>117</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="3">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <f>N2-SUM(I2:I6)</f>
+        <v>101</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <f>N3-SUM(I7:I12)</f>
+        <v>89</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="3">
+        <v>4</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <f>N4-SUM(I13:I17)</f>
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="O5" s="3"/>
+      <c r="P5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <f>N5-SUM(I18:I21)</f>
+        <v>64</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
+      <c r="N7" s="3">
+        <f>N6-SUM(I22:I26)</f>
+        <v>47</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3">
+        <f>N7-SUM(I27:I29)</f>
+        <v>30</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3">
+        <f>N8-SUM(I30)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="3">
+        <v>5</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" t="s">
-        <v>74</v>
-      </c>
+      <c r="I16" s="3">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="3">
+        <v>5</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="3">
+        <v>4</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="3">
+        <v>2</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="3">
+        <v>4</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="3">
+        <v>4</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="3">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29">
+        <v>30</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="3">
+        <v>10</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" s="3">
+        <v>30</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I31" s="3">
+        <f>SUM(C2:C30)</f>
+        <v>117</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3C4868-DA68-4B79-A75F-C29998123D8F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cuncurency, backlog and mvc updated
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="195">
   <si>
     <t>Play song</t>
   </si>
@@ -603,6 +603,12 @@
   </si>
   <si>
     <t>Report planning</t>
+  </si>
+  <si>
+    <t>Get 10 messages at a time</t>
+  </si>
+  <si>
+    <t>Joined chat between web/dedicated</t>
   </si>
 </sst>
 </file>
@@ -2390,7 +2396,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$C$22</c:f>
+              <c:f>'Sprint 4'!$C$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2454,33 +2460,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$D$22:$L$22</c:f>
+              <c:f>'Sprint 4'!$D$24:$L$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.5</c:v>
+                  <c:v>92.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.5</c:v>
+                  <c:v>66.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.5</c:v>
+                  <c:v>39.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.5</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2500,7 +2506,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$C$23</c:f>
+              <c:f>'Sprint 4'!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2564,7 +2570,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$D$23:$L$23</c:f>
+              <c:f>'Sprint 4'!$D$25:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -10661,7 +10667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2037159B-319A-4C42-A294-2B2489B57574}">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -12045,27 +12051,27 @@
         <v>155</v>
       </c>
       <c r="D33" s="4">
-        <f>SUM(D2:D31)</f>
+        <f t="shared" ref="D33:I33" si="1">SUM(D2:D31)</f>
         <v>90</v>
       </c>
       <c r="E33" s="4">
-        <f>SUM(E2:E31)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="F33" s="4">
-        <f>SUM(F2:F31)</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="G33" s="4">
-        <f>SUM(G2:G31)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="H33" s="4">
-        <f>SUM(H2:H31)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I33" s="4">
-        <f>SUM(I2:I31)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -12240,8 +12246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7884E-D22C-4C15-B48F-DDAEB03C83F5}">
   <dimension ref="A1:X64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:D62"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13620,31 +13626,31 @@
         <v>110</v>
       </c>
       <c r="E30" s="4">
-        <f>D30-($D$30/7)</f>
+        <f t="shared" ref="E30:K30" si="0">D30-($D$30/7)</f>
         <v>94.285714285714292</v>
       </c>
       <c r="F30" s="4">
-        <f>E30-($D$30/7)</f>
+        <f t="shared" si="0"/>
         <v>78.571428571428584</v>
       </c>
       <c r="G30" s="4">
-        <f>F30-($D$30/7)</f>
+        <f t="shared" si="0"/>
         <v>62.857142857142868</v>
       </c>
       <c r="H30" s="4">
-        <f>G30-($D$30/7)</f>
+        <f t="shared" si="0"/>
         <v>47.142857142857153</v>
       </c>
       <c r="I30" s="4">
-        <f>H30-($D$30/7)</f>
+        <f t="shared" si="0"/>
         <v>31.428571428571438</v>
       </c>
       <c r="J30" s="4">
-        <f>I30-($D$30/7)</f>
+        <f t="shared" si="0"/>
         <v>15.714285714285724</v>
       </c>
       <c r="K30" s="4">
-        <f>J30-($D$30/7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L30" s="4"/>
@@ -13664,31 +13670,31 @@
         <v>108</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" ref="E31:K31" si="0">SUM(E2:E29)</f>
+        <f t="shared" ref="E31:K31" si="1">SUM(E2:E29)</f>
         <v>107</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="L31" s="4"/>
@@ -13884,10 +13890,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3C4868-DA68-4B79-A75F-C29998123D8F}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13899,6 +13905,7 @@
     <col min="9" max="9" width="11.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14248,86 +14255,108 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
+    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="4">
-        <f>SUM(C2:C21)</f>
-        <v>100</v>
-      </c>
-      <c r="E22" s="4">
-        <f>D22-($D$22/8)</f>
-        <v>87.5</v>
-      </c>
-      <c r="F22" s="4">
-        <f>E22-($D$22/8)</f>
-        <v>75</v>
-      </c>
-      <c r="G22" s="4">
-        <f>F22-($D$22/8)</f>
-        <v>62.5</v>
-      </c>
-      <c r="H22" s="4">
-        <f>G22-($D$22/8)</f>
-        <v>50</v>
-      </c>
-      <c r="I22" s="4">
-        <f>H22-($D$22/8)</f>
-        <v>37.5</v>
-      </c>
-      <c r="J22" s="4">
-        <f>I22-($D$22/8)</f>
-        <v>25</v>
-      </c>
-      <c r="K22" s="4">
-        <f>J22-($D$22/8)</f>
-        <v>12.5</v>
-      </c>
-      <c r="L22" s="4">
-        <f>K22-($D$22/8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="4">
+        <f>SUM(C2:C23)</f>
+        <v>106</v>
+      </c>
+      <c r="E24" s="4">
+        <f>D24-($D$24/8)</f>
+        <v>92.75</v>
+      </c>
+      <c r="F24" s="4">
+        <f>E24-($D$24/8)</f>
+        <v>79.5</v>
+      </c>
+      <c r="G24" s="4">
+        <f>F24-($D$24/8)</f>
+        <v>66.25</v>
+      </c>
+      <c r="H24" s="4">
+        <f>G24-($D$24/8)</f>
+        <v>53</v>
+      </c>
+      <c r="I24" s="4">
+        <f>H24-($D$24/8)</f>
+        <v>39.75</v>
+      </c>
+      <c r="J24" s="4">
+        <f>I24-($D$24/8)</f>
+        <v>26.5</v>
+      </c>
+      <c r="K24" s="4">
+        <f>J24-($D$24/8)</f>
+        <v>13.25</v>
+      </c>
+      <c r="L24" s="4">
+        <f>K24-($D$24/8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="4">
-        <f>SUM(D2:D21)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <f>SUM(E2:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="4">
-        <f>SUM(F2:F21)</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <f>SUM(G2:G21)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <f>SUM(H2:H21)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <f>SUM(I2:I21)</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="4">
-        <f>SUM(J2:J21)</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
-        <f>SUM(K2:K21)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
-        <f>SUM(L2:L21)</f>
+      <c r="D25" s="4">
+        <f>SUM(D2:D23)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" ref="E25:L25" si="0">SUM(E2:E23)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating sprint tables in sysdev report
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -667,7 +667,7 @@
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -685,7 +685,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -932,7 +932,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -976,7 +976,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -1017,7 +1017,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1057,7 +1057,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1071,7 +1071,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1414,7 +1414,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -1458,7 +1458,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -1499,7 +1499,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1539,7 +1539,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1553,7 +1553,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1800,7 +1800,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -1844,7 +1844,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -1885,7 +1885,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1925,7 +1925,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1939,7 +1939,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2210,7 +2210,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -2279,7 +2279,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -2320,7 +2320,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2360,7 +2360,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2374,7 +2374,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2657,7 +2657,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -2726,7 +2726,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -2767,7 +2767,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2807,7 +2807,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5974,6 +5974,92 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78447A4E-CDB3-45EE-91A3-4EA22F56CF94}" name="Table2" displayName="Table2" ref="A1:J21" totalsRowShown="0">
+  <autoFilter ref="A1:J21" xr:uid="{C94A59BC-04BB-4AF5-9E59-80489801E0B2}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{03317E6F-5E64-493A-8CF3-61F18B436878}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{98825976-954F-479D-8108-396FEA9CA78A}" name="Work"/>
+    <tableColumn id="3" xr3:uid="{17ECD59D-0031-4A1B-B29F-E0E0CFB6C093}" name="time-est."/>
+    <tableColumn id="4" xr3:uid="{ADF84FA0-4D7F-4111-8508-929E463CAE1B}" name="25.10.2017"/>
+    <tableColumn id="5" xr3:uid="{BA314F50-6242-4633-9060-7BA63BF5F30E}" name="26.10.2017"/>
+    <tableColumn id="6" xr3:uid="{8AB26860-FC22-4A20-BE25-981489E8D4AA}" name="27.10.2017"/>
+    <tableColumn id="7" xr3:uid="{78B906B5-4501-4375-A5F0-A8019DA52149}" name="31.10.2017"/>
+    <tableColumn id="8" xr3:uid="{5F101E0C-ABBD-4941-A078-4CFF0A6B631F}" name="3.11.2017"/>
+    <tableColumn id="9" xr3:uid="{04063FC7-24F4-417A-86E7-F3960DB84B71}" name="6.11.2017"/>
+    <tableColumn id="10" xr3:uid="{FD179364-17E0-4BE6-A1D6-B849331A4B2C}" name="Person"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3FF0DD1C-4E49-4E7F-92CA-CB567AA3CB8E}" name="Table3" displayName="Table3" ref="A1:R33" totalsRowShown="0">
+  <autoFilter ref="A1:R33" xr:uid="{A001DDB7-4D03-41B6-A7CC-449892123C18}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{630B2E25-8E62-4D5D-AC40-3F67A507481F}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{E464CF59-1F40-432D-805D-D490D95510DD}" name="Work"/>
+    <tableColumn id="3" xr3:uid="{4B44EF22-B40A-44E1-9DA3-DE04BD21156E}" name="time-est."/>
+    <tableColumn id="4" xr3:uid="{60BB57D2-D349-441D-82A7-E0981FE04683}" name="8.11.2017"/>
+    <tableColumn id="5" xr3:uid="{3D5C7D68-C2F5-4A6A-971D-2E85D65F9867}" name="9.11.2017"/>
+    <tableColumn id="6" xr3:uid="{FE2C541D-8359-45A3-9CCF-5753C8A87EEF}" name="10.11.2017"/>
+    <tableColumn id="7" xr3:uid="{5FC0FACB-14F9-4A58-A454-5C2D470B83D3}" name="11.11.2017"/>
+    <tableColumn id="8" xr3:uid="{1C2025F8-27E6-44B2-A26A-6266F504CB1A}" name="12.11.2017"/>
+    <tableColumn id="9" xr3:uid="{A7FB4B68-F13B-4515-96CB-5F810B5B5ECB}" name="13.11.2017"/>
+    <tableColumn id="10" xr3:uid="{B64F9B56-D82D-4842-8B5F-74BE82D4E7F1}" name="14.11.2017"/>
+    <tableColumn id="11" xr3:uid="{B16195A0-E19D-4539-90AB-FCFFBAD25B0A}" name="15.11.2017"/>
+    <tableColumn id="12" xr3:uid="{1D17ECC7-1F51-4411-BBE6-D0AD1B5CF65B}" name="16.11.2017"/>
+    <tableColumn id="13" xr3:uid="{29DF574E-AF6C-46F5-8D08-458681778AC6}" name="17.11.2017"/>
+    <tableColumn id="14" xr3:uid="{4800A496-3370-40FF-AEC6-4A134FD11701}" name="18.11.2017"/>
+    <tableColumn id="15" xr3:uid="{AF3D249D-BE14-49A9-836B-2D4B8A084691}" name="19.11.2017"/>
+    <tableColumn id="16" xr3:uid="{9D2BF2D6-4506-449A-AE26-EEF5B2CE6306}" name="20.11.2017"/>
+    <tableColumn id="17" xr3:uid="{708A7FB6-A228-462A-80A8-01629604BBC5}" name="21.11.2017"/>
+    <tableColumn id="18" xr3:uid="{7E7DE8B1-6FE9-4C69-99B7-6A0BEEA23054}" name="Person"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6040D3C7-704D-4B34-9CD1-FCC83E772A66}" name="Table4" displayName="Table4" ref="A1:J31" totalsRowShown="0">
+  <autoFilter ref="A1:J31" xr:uid="{ACD998EF-9F68-4272-9D9B-C9575E3BBCF2}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{DB80EF25-AB96-4C8A-947A-9698EAA200D0}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{3A78EDAA-6898-4E45-8503-D686A2CE064F}" name="Work"/>
+    <tableColumn id="3" xr3:uid="{6D5E5F6C-9FAA-4FF3-AE1A-9AB2E5D93FFF}" name="time-est."/>
+    <tableColumn id="4" xr3:uid="{624AEDA0-C87E-466A-B79B-F052A960261C}" name="22.11.2017"/>
+    <tableColumn id="5" xr3:uid="{B8A2D6E7-BE4C-4402-B763-2492709AFA03}" name="23.11.2017"/>
+    <tableColumn id="6" xr3:uid="{F1719CD4-79DC-4FD8-9BF3-2A3BB701D0A1}" name="24.11.2017"/>
+    <tableColumn id="7" xr3:uid="{635529AE-16E7-4138-AE9E-73C1ECC43B46}" name="25.11.2017"/>
+    <tableColumn id="8" xr3:uid="{38C25D8D-9330-4741-A988-74ACB936E276}" name="26.11.2017"/>
+    <tableColumn id="9" xr3:uid="{D85D4688-5066-4445-8F81-75B3F83892E8}" name="27.11.2017"/>
+    <tableColumn id="10" xr3:uid="{4461199D-5506-46DE-8D4D-8B8CFDE54FC3}" name="Person"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{485FC9A2-2ECA-4867-B849-A896468FE32C}" name="Table1" displayName="Table1" ref="A1:L29" totalsRowShown="0">
+  <autoFilter ref="A1:L29" xr:uid="{2C3F92BE-8B09-468B-934C-DB92BECE08EA}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{9880F961-2E97-46DB-8F7D-08DD7C0BF047}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{FED33286-50D6-44CD-BC0A-6D6E4CCBA7B7}" name="Work"/>
+    <tableColumn id="3" xr3:uid="{638EF93A-44EE-40EB-BB12-4EDCBA47B63F}" name="time-est."/>
+    <tableColumn id="4" xr3:uid="{0E38524A-6FEC-46D6-A81B-5FD52AA91222}" name="28.11.2017"/>
+    <tableColumn id="5" xr3:uid="{9A84DAA7-1B55-4406-AFE2-BC5EBB40F2B6}" name="29.11.2017"/>
+    <tableColumn id="6" xr3:uid="{8E2EA95B-3C25-4733-BAFC-214CD135B888}" name="30.11.2017"/>
+    <tableColumn id="7" xr3:uid="{52452300-D7CD-433B-9646-BF6B754E30E5}" name="1.12.2017"/>
+    <tableColumn id="8" xr3:uid="{0C2C69C9-0839-458B-BB2B-FBF9EB9EEC73}" name="2.12.2017"/>
+    <tableColumn id="9" xr3:uid="{DD6E818E-6444-40CF-98CB-1A3CE46971D6}" name="3.12.2017"/>
+    <tableColumn id="10" xr3:uid="{DB5CE761-C263-44FE-944D-42EEA0D414F5}" name="4.12.2017"/>
+    <tableColumn id="11" xr3:uid="{D12129C4-1D29-4D8A-857F-9EFDCD56F08B}" name="5.12.2017"/>
+    <tableColumn id="12" xr3:uid="{A8FC9E0B-9761-42A6-8218-479E5D4A44F3}" name="Person"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7268,19 +7354,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416D8BE7-F174-4DE6-8BD7-669440759E00}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D46"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="4" customWidth="1"/>
+    <col min="4" max="6" width="15.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="13.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8183,6 +8269,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -8190,17 +8279,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView topLeftCell="I22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:D70"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R33" sqref="A1:R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="4" customWidth="1"/>
+    <col min="5" max="15" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="4" customWidth="1"/>
     <col min="17" max="17" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -10660,6 +10752,9 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -10668,14 +10763,15 @@
   <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection sqref="A1:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.140625" style="4" customWidth="1"/>
+    <col min="4" max="9" width="15.28515625" style="4" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -12239,6 +12335,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12247,16 +12346,17 @@
   <dimension ref="A1:X64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.28515625" style="4" customWidth="1"/>
+    <col min="7" max="10" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="4" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -13885,6 +13985,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -13892,7 +13995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3C4868-DA68-4B79-A75F-C29998123D8F}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -14286,35 +14389,35 @@
         <v>106</v>
       </c>
       <c r="E24" s="4">
-        <f>D24-($D$24/8)</f>
+        <f t="shared" ref="E24:L24" si="0">D24-($D$24/8)</f>
         <v>92.75</v>
       </c>
       <c r="F24" s="4">
-        <f>E24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>79.5</v>
       </c>
       <c r="G24" s="4">
-        <f>F24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>66.25</v>
       </c>
       <c r="H24" s="4">
-        <f>G24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="I24" s="4">
-        <f>H24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>39.75</v>
       </c>
       <c r="J24" s="4">
-        <f>I24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>26.5</v>
       </c>
       <c r="K24" s="4">
-        <f>J24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>13.25</v>
       </c>
       <c r="L24" s="4">
-        <f>K24-($D$24/8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -14328,35 +14431,35 @@
         <v>0</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" ref="E25:L25" si="0">SUM(E2:E23)</f>
+        <f t="shared" ref="E25:L25" si="1">SUM(E2:E23)</f>
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
domain model, sprint backlog and mvc chat changed
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="212">
   <si>
     <t>Play song</t>
   </si>
@@ -287,9 +287,6 @@
     <t>Game debug/release mode execution error</t>
   </si>
   <si>
-    <t>Refactor database</t>
-  </si>
-  <si>
     <t>Exception handling</t>
   </si>
   <si>
@@ -323,9 +320,6 @@
     <t>Development Method of Choice</t>
   </si>
   <si>
-    <t>merging Report</t>
-  </si>
-  <si>
     <t>Giving feedback on report</t>
   </si>
   <si>
@@ -566,9 +560,6 @@
     <t>Signalr spike</t>
   </si>
   <si>
-    <t>Sprint sum-up</t>
-  </si>
-  <si>
     <t>Report planning</t>
   </si>
   <si>
@@ -590,30 +581,9 @@
     <t>Read about chats (how to make)</t>
   </si>
   <si>
-    <t>Database model 1st. Version</t>
-  </si>
-  <si>
-    <t>Domain model 1st. Version</t>
-  </si>
-  <si>
     <t>Update problem statement</t>
   </si>
   <si>
-    <t>Update domain model (add song and playlist)</t>
-  </si>
-  <si>
-    <t>Update database (add song and playlist)</t>
-  </si>
-  <si>
-    <t>Update database diagram</t>
-  </si>
-  <si>
-    <t>Update database diagram (add song and playlist)</t>
-  </si>
-  <si>
-    <t>Finish Domain model (Optimize profile)</t>
-  </si>
-  <si>
     <t>Fix and create more tests</t>
   </si>
   <si>
@@ -647,13 +617,49 @@
     <t>Review and if necessary fix backlog</t>
   </si>
   <si>
-    <t>Reoprt review</t>
-  </si>
-  <si>
     <t>Finalize MVC (mvc chat and login)</t>
   </si>
   <si>
     <t>Finish MoSCoW model</t>
+  </si>
+  <si>
+    <t>Domain model (chat and profile)</t>
+  </si>
+  <si>
+    <t>Database model (chat and profile)</t>
+  </si>
+  <si>
+    <t>Update database and add (song and playlist)</t>
+  </si>
+  <si>
+    <t>Update database diagram and add (song and playlist)</t>
+  </si>
+  <si>
+    <t>Update database and add (group)</t>
+  </si>
+  <si>
+    <t>Update database diagram and add (group)</t>
+  </si>
+  <si>
+    <t>Update domain model and add (group)</t>
+  </si>
+  <si>
+    <t>Sprint sum-up (until now)</t>
+  </si>
+  <si>
+    <t>Dedicated client (for existing functionality)</t>
+  </si>
+  <si>
+    <t>Sprint sum-up (final)</t>
+  </si>
+  <si>
+    <t>Report review</t>
+  </si>
+  <si>
+    <t>Merging Report</t>
+  </si>
+  <si>
+    <t>Update domain model and add (song,  playlist, notifications)</t>
   </si>
 </sst>
 </file>
@@ -714,7 +720,11 @@
   <cellStyles count="1">
     <cellStyle name="Parasts" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -898,19 +908,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>103</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.4</c:v>
+                  <c:v>76.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.800000000000004</c:v>
+                  <c:v>57.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.2</c:v>
+                  <c:v>38.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.6</c:v>
+                  <c:v>19.199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -990,19 +1000,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>98</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
@@ -2180,19 +2190,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76</c:v>
+                  <c:v>74.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>55.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2272,7 +2282,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>93</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70</c:v>
@@ -3242,7 +3252,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$C$22</c:f>
+              <c:f>'Sprint 4'!$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3306,33 +3316,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$D$22:$L$22</c:f>
+              <c:f>'Sprint 4'!$D$23:$L$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>94</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.25</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.5</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.75</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.25</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.75</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3352,7 +3362,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 4'!$C$23</c:f>
+              <c:f>'Sprint 4'!$C$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3416,18 +3426,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$D$23:$L$23</c:f>
+              <c:f>'Sprint 4'!$D$24:$L$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>62</c:v>
@@ -6787,7 +6797,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>176892</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6873,7 +6883,7 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>309283</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6985,6 +6995,28 @@
     <tableColumn id="10" xr3:uid="{DB5CE761-C263-44FE-944D-42EEA0D414F5}" name="4.12.2017"/>
     <tableColumn id="11" xr3:uid="{D12129C4-1D29-4D8A-857F-9EFDCD56F08B}" name="5.12.2017"/>
     <tableColumn id="12" xr3:uid="{A8FC9E0B-9761-42A6-8218-479E5D4A44F3}" name="Person"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{69F42748-5731-45AD-AB2F-2D56CE6CE30F}" name="Tabula5" displayName="Tabula5" ref="A1:M22" totalsRowShown="0">
+  <autoFilter ref="A1:M22" xr:uid="{53754D2A-1621-4F83-9B64-281BB9D7345E}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{306EE1EA-B0B1-4175-8E88-A2B100506FAC}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{4DF1E167-2B6E-4646-9E57-BBD0A536C003}" name="Work" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{FF972DE1-AB0B-4929-98A7-EF76BB4B4F75}" name="time-est."/>
+    <tableColumn id="4" xr3:uid="{E0A23C63-298C-4EE0-B937-0CE2842AEF13}" name="5.12.2017"/>
+    <tableColumn id="5" xr3:uid="{06523220-F482-4E4F-80DF-AF0B07E8008D}" name="6.12.2017"/>
+    <tableColumn id="6" xr3:uid="{F42B1C34-8E39-4DC4-812D-74DB150E1376}" name="7.12.2017"/>
+    <tableColumn id="7" xr3:uid="{F8E2A858-D2A3-4E58-BF20-04FFF947CA18}" name="8.12.2017"/>
+    <tableColumn id="8" xr3:uid="{591CA4B6-29BF-4E1C-B96F-D6DD1DF9437E}" name="9.12.2017"/>
+    <tableColumn id="9" xr3:uid="{8FCC6452-56F4-4BEF-935B-9250EDB59435}" name="10.12.2017"/>
+    <tableColumn id="10" xr3:uid="{14D28F79-F9A0-4876-8542-24D8499B8C69}" name="11.12.2017"/>
+    <tableColumn id="11" xr3:uid="{DC40776A-5787-419C-BE3E-815487055AB1}" name="12.12.2017"/>
+    <tableColumn id="12" xr3:uid="{A690D3DE-F147-4B4E-9360-A2B2A43A33D2}" name="13.12.2017"/>
+    <tableColumn id="13" xr3:uid="{945433BC-B052-4280-81C3-8CFCBAC7FAF9}" name="Person"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7255,8 +7287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7341,7 +7373,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -7369,7 +7401,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C8">
         <v>80</v>
@@ -7957,7 +7989,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C49" s="4">
         <v>1</v>
@@ -8283,7 +8315,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8309,22 +8341,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -8344,7 +8376,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -8420,7 +8452,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8496,7 +8528,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
@@ -8636,7 +8668,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -8735,7 +8767,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C13" s="4">
         <v>3</v>
@@ -8869,7 +8901,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -8901,7 +8933,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
@@ -8933,25 +8965,25 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D19" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E19" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F19" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I19" s="4">
         <v>0</v>
@@ -8997,25 +9029,25 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E21" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F21" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G21" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H21" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
@@ -9122,27 +9154,27 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D25" s="4">
         <f>SUM(C2:C24)</f>
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E25" s="4">
         <f>D25-($D$25/5)</f>
-        <v>82.4</v>
+        <v>76.8</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" ref="F25:I25" si="0">E25-($D$25/5)</f>
-        <v>61.800000000000004</v>
+        <v>57.599999999999994</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>41.2</v>
+        <v>38.399999999999991</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>20.6</v>
+        <v>19.199999999999992</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="0"/>
@@ -9151,27 +9183,27 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" ref="D26:I26" si="1">SUM(D2:D24)</f>
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I26" s="4">
         <f t="shared" si="1"/>
@@ -9306,14 +9338,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
   <dimension ref="A1:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="4" customWidth="1"/>
     <col min="5" max="15" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -9336,46 +9368,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="R1" t="s">
         <v>3</v>
@@ -9774,7 +9806,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -10894,7 +10926,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
@@ -11220,7 +11252,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>207</v>
       </c>
       <c r="C30">
         <v>25</v>
@@ -11280,10 +11312,10 @@
     </row>
     <row r="31" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="C31" s="4">
         <v>3</v>
@@ -11343,10 +11375,10 @@
     </row>
     <row r="32" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C32" s="4">
         <v>2</v>
@@ -11406,10 +11438,10 @@
     </row>
     <row r="33" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -11472,7 +11504,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C34" s="4">
         <v>3</v>
@@ -11532,7 +11564,7 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D35" s="4">
         <f>SUM(C2:C34)</f>
@@ -11600,7 +11632,7 @@
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D36" s="4">
         <f>SUM(D2:D34)</f>
@@ -11846,7 +11878,7 @@
   <dimension ref="A1:X72"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11870,22 +11902,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -12174,7 +12206,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -12219,7 +12251,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
@@ -12429,25 +12461,25 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>87</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G14" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
@@ -12461,7 +12493,8 @@
       <c r="K14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -12469,27 +12502,27 @@
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
+    <row r="15" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
       </c>
       <c r="D15" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4">
         <v>0</v>
@@ -12497,13 +12530,12 @@
       <c r="I15" s="4">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="4"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -12512,21 +12544,21 @@
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16">
+    <row r="16" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="4">
         <v>2</v>
       </c>
       <c r="D16" s="4">
         <v>2</v>
       </c>
       <c r="E16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -12540,13 +12572,13 @@
       <c r="I16" s="4">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
-        <v>37</v>
+      <c r="J16" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -12556,16 +12588,16 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>87</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -12595,16 +12627,13 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -12649,7 +12678,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -12658,7 +12687,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -12678,8 +12707,7 @@
       <c r="K19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="2"/>
+      <c r="M19" s="4"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -12695,7 +12723,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -12741,7 +12769,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -12787,7 +12815,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -12829,13 +12857,13 @@
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" s="4">
@@ -12856,11 +12884,14 @@
       <c r="I23" s="4">
         <v>0</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -12876,7 +12907,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -12919,16 +12950,16 @@
         <v>2</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>200</v>
+        <v>29</v>
       </c>
       <c r="C25" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <v>0</v>
@@ -12957,24 +12988,24 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C26" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26" s="4">
         <v>0</v>
@@ -12988,6 +13019,8 @@
       <c r="J26" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="K26" s="4"/>
+      <c r="M26" s="4"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -12998,24 +13031,24 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>35</v>
+        <v>191</v>
       </c>
       <c r="C27" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="4">
         <v>0</v>
@@ -13029,8 +13062,6 @@
       <c r="J27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="M27" s="4"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -13043,22 +13074,22 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C28" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D28" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E28" s="4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F28" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G28" s="4">
         <v>0</v>
@@ -13072,8 +13103,8 @@
       <c r="J28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="1"/>
-      <c r="M28" s="2"/>
+      <c r="K28" s="4"/>
+      <c r="M28" s="4"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -13086,22 +13117,22 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>199</v>
+        <v>33</v>
       </c>
       <c r="C29" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D29" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E29" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G29" s="4">
         <v>0</v>
@@ -13115,8 +13146,7 @@
       <c r="J29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
+      <c r="K29" s="1"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -13133,7 +13163,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
@@ -13142,7 +13172,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30" s="4">
         <v>0</v>
@@ -13165,25 +13195,31 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
+      <c r="A31" s="4">
+        <v>2</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
       </c>
       <c r="D31" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E31" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G31" s="4">
         <v>0</v>
@@ -13194,33 +13230,34 @@
       <c r="I31" s="4">
         <v>0</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="1"/>
+      <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-    </row>
-    <row r="32" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>1</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C32" s="4">
-        <v>1</v>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
       </c>
       <c r="D32" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F32" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G32" s="4">
         <v>0</v>
@@ -13231,10 +13268,11 @@
       <c r="I32" s="4">
         <v>0</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" t="s">
         <v>38</v>
       </c>
       <c r="K32" s="1"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -13244,10 +13282,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="C33" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
@@ -13280,7 +13318,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C34">
         <v>18</v>
@@ -13314,7 +13352,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -13346,27 +13384,27 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D36" s="4">
         <f>SUM(C2:C35)</f>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E36" s="4">
         <f>D36-($D$36/5)</f>
-        <v>76</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="F36" s="4">
         <f t="shared" ref="F36:I36" si="0">E36-($D$36/5)</f>
-        <v>57</v>
+        <v>55.800000000000004</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="0"/>
@@ -13378,11 +13416,11 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" ref="D37:I37" si="1">SUM(D2:D35)</f>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" si="1"/>
@@ -13579,14 +13617,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7884E-D22C-4C15-B48F-DDAEB03C83F5}">
   <dimension ref="A1:X65"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="15.28515625" style="4" customWidth="1"/>
     <col min="7" max="10" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -13609,28 +13647,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
@@ -13811,7 +13849,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -13863,7 +13901,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -13915,7 +13953,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -13967,7 +14005,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -14017,7 +14055,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -14067,7 +14105,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -14117,7 +14155,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -14167,7 +14205,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -14217,7 +14255,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -14267,7 +14305,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -14317,7 +14355,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -14364,7 +14402,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -14408,7 +14446,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -14452,7 +14490,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -14496,7 +14534,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -14540,7 +14578,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -14581,7 +14619,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -14622,7 +14660,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -14663,7 +14701,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -14704,7 +14742,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -14745,7 +14783,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -14786,7 +14824,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -14827,7 +14865,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -14868,7 +14906,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C28">
         <v>25</v>
@@ -14912,7 +14950,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -14950,7 +14988,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C30" s="4">
         <v>4</v>
@@ -14991,7 +15029,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D31" s="4">
         <f>SUM(C2:C30)</f>
@@ -15035,7 +15073,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" ref="D32:K32" si="1">SUM(D2:D30)</f>
@@ -15265,22 +15303,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3C4868-DA68-4B79-A75F-C29998123D8F}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="8" width="14.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" style="4" customWidth="1"/>
+    <col min="11" max="12" width="15.28515625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15295,31 +15334,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>173</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>3</v>
@@ -15333,7 +15372,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -15374,7 +15413,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -15415,7 +15454,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -15456,7 +15495,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -15497,7 +15536,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -15538,7 +15577,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -15579,7 +15618,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -15623,7 +15662,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -15667,7 +15706,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -15710,8 +15749,8 @@
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
-        <v>131</v>
+      <c r="B11" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -15755,7 +15794,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -15799,7 +15838,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -15843,7 +15882,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C14" s="4">
         <v>4</v>
@@ -15882,30 +15921,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>1</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
+        <v>208</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
         <v>2</v>
       </c>
       <c r="E15" s="4">
         <v>2</v>
       </c>
       <c r="F15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
@@ -15920,33 +15959,36 @@
         <v>0</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>66</v>
+        <v>38</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>137</v>
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G16" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" s="4">
         <v>0</v>
@@ -15966,25 +16008,25 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>138</v>
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G17" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" s="4">
         <v>0</v>
@@ -16009,14 +16051,14 @@
       <c r="A18">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
-        <v>139</v>
+      <c r="B18" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -16050,23 +16092,23 @@
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>175</v>
+      <c r="B19" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="4">
         <v>0</v>
@@ -16092,190 +16134,225 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
+        <v>4</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21">
         <v>20</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D21" s="4">
         <v>20</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E21" s="4">
         <v>16</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F21" s="4">
         <v>15</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G21" s="4">
         <v>13</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H21" s="4">
         <v>10</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I21" s="4">
         <v>7</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J21" s="4">
         <v>5</v>
       </c>
-      <c r="K20" s="4">
-        <v>3</v>
-      </c>
-      <c r="L20" s="4">
-        <v>1</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>2</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C21" s="4">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4">
-        <v>4</v>
-      </c>
-      <c r="G21" s="4">
-        <v>4</v>
-      </c>
-      <c r="H21" s="4">
-        <v>4</v>
-      </c>
-      <c r="I21" s="4">
-        <v>4</v>
-      </c>
-      <c r="J21" s="4">
-        <v>7</v>
-      </c>
       <c r="K21" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
-        <v>144</v>
+    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="4">
+        <v>4</v>
       </c>
       <c r="D22" s="4">
-        <f>SUM(C2:C21)</f>
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" ref="E22:L22" si="0">D22-($D$22/8)</f>
-        <v>82.25</v>
+        <v>4</v>
       </c>
       <c r="F22" s="4">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>4</v>
+      </c>
+      <c r="H22" s="4">
+        <v>4</v>
+      </c>
+      <c r="I22" s="4">
+        <v>4</v>
+      </c>
+      <c r="J22" s="4">
+        <v>7</v>
+      </c>
+      <c r="K22" s="4">
+        <v>6</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(C2:C22)</f>
+        <v>96</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" ref="E23:L23" si="0">D23-($D$23/8)</f>
+        <v>84</v>
+      </c>
+      <c r="F23" s="4">
         <f t="shared" si="0"/>
-        <v>70.5</v>
-      </c>
-      <c r="G22" s="4">
+        <v>72</v>
+      </c>
+      <c r="G23" s="4">
         <f t="shared" si="0"/>
-        <v>58.75</v>
-      </c>
-      <c r="H22" s="4">
+        <v>60</v>
+      </c>
+      <c r="H23" s="4">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="I22" s="4">
+        <v>48</v>
+      </c>
+      <c r="I23" s="4">
         <f t="shared" si="0"/>
-        <v>35.25</v>
-      </c>
-      <c r="J22" s="4">
+        <v>36</v>
+      </c>
+      <c r="J23" s="4">
         <f t="shared" si="0"/>
-        <v>23.5</v>
-      </c>
-      <c r="K22" s="4">
+        <v>24</v>
+      </c>
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
-        <v>11.75</v>
-      </c>
-      <c r="L22" s="4">
+        <v>12</v>
+      </c>
+      <c r="L23" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="4">
-        <f>SUM(D2:D21)</f>
-        <v>95</v>
-      </c>
-      <c r="E23" s="4">
-        <f t="shared" ref="E23:L23" si="1">SUM(E2:E21)</f>
-        <v>90</v>
-      </c>
-      <c r="F23" s="4">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="4">
+        <f>SUM(D2:D22)</f>
+        <v>97</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" ref="E24:L24" si="1">SUM(E2:E22)</f>
+        <v>92</v>
+      </c>
+      <c r="F24" s="4">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="G23" s="4">
+        <v>82</v>
+      </c>
+      <c r="G24" s="4">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H24" s="4">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I24" s="4">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J24" s="4">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K24" s="4">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L24" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>182</v>
+      <c r="B28" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
@@ -16317,61 +16394,61 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
+      <c r="B47" s="5"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
+      <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
@@ -16381,9 +16458,18 @@
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
model layer classes are extending activity (message, group, chat), design class diagram up to date, domain model updated and backlog updated
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="211">
   <si>
     <t>Play song</t>
   </si>
@@ -566,9 +566,6 @@
     <t>use activity model layer class</t>
   </si>
   <si>
-    <t>make chat work on web client</t>
-  </si>
-  <si>
     <t>Create Mock up</t>
   </si>
   <si>
@@ -617,18 +614,9 @@
     <t>Review and if necessary fix backlog</t>
   </si>
   <si>
-    <t>Finalize MVC (mvc chat and login)</t>
-  </si>
-  <si>
     <t>Finish MoSCoW model</t>
   </si>
   <si>
-    <t>Domain model (chat and profile)</t>
-  </si>
-  <si>
-    <t>Database model (chat and profile)</t>
-  </si>
-  <si>
     <t>Update database and add (song and playlist)</t>
   </si>
   <si>
@@ -660,6 +648,15 @@
   </si>
   <si>
     <t>Update domain model and add (song,  playlist, notifications)</t>
+  </si>
+  <si>
+    <t>Finalize MVC (chat and login)</t>
+  </si>
+  <si>
+    <t>Database model (chat, message, profile)</t>
+  </si>
+  <si>
+    <t>Domain model (chat, message,  profile)</t>
   </si>
 </sst>
 </file>
@@ -8314,14 +8311,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416D8BE7-F174-4DE6-8BD7-669440759E00}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="15.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="4" customWidth="1"/>
@@ -8376,7 +8373,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -8452,7 +8449,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -8767,7 +8764,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="4">
         <v>3</v>
@@ -8901,7 +8898,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -8933,7 +8930,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
@@ -8965,7 +8962,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -9029,7 +9026,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -9338,7 +9335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F0FA56-3052-4FDF-A416-31284BD45B6D}">
   <dimension ref="A1:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -10926,7 +10923,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
@@ -11252,7 +11249,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C30">
         <v>25</v>
@@ -11315,7 +11312,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C31" s="4">
         <v>3</v>
@@ -11378,7 +11375,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C32" s="4">
         <v>2</v>
@@ -11441,7 +11438,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -11504,7 +11501,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C34" s="4">
         <v>3</v>
@@ -12251,7 +12248,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
@@ -12507,7 +12504,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
@@ -12549,7 +12546,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C16" s="4">
         <v>2</v>
@@ -12633,7 +12630,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -12678,7 +12675,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -12993,7 +12990,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
@@ -13036,7 +13033,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -13163,7 +13160,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C30" s="4">
         <v>1</v>
@@ -13282,7 +13279,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -13352,7 +13349,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -14783,7 +14780,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -14906,7 +14903,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C28">
         <v>25</v>
@@ -14988,7 +14985,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C30" s="4">
         <v>4</v>
@@ -15306,7 +15303,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15372,7 +15369,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -15882,7 +15879,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" s="4">
         <v>4</v>
@@ -15926,7 +15923,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
@@ -16175,7 +16172,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -16216,7 +16213,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C22" s="4">
         <v>4</v>
@@ -16346,9 +16343,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>

</xml_diff>

<commit_message>
sys dev and tech report updates
</commit_message>
<xml_diff>
--- a/project/SystemDev/Sprint_Backlog.xlsx
+++ b/project/SystemDev/Sprint_Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Time est.</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -651,6 +648,9 @@
   </si>
   <si>
     <t>Design class diagram(for report)</t>
+  </si>
+  <si>
+    <t>Time est. (hours)</t>
   </si>
 </sst>
 </file>
@@ -686,32 +686,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Parasts" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -934,6 +919,24 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -955,7 +958,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1048,7 +1051,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1311,7 +1314,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1342,7 +1345,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -1466,7 +1469,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1497,7 +1500,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -1548,7 +1551,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1562,7 +1565,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1627,7 +1630,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1986,7 +1989,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2017,7 +2020,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -2141,7 +2144,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2172,7 +2175,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -2223,7 +2226,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2237,7 +2240,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2330,7 +2333,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2593,7 +2596,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2624,7 +2627,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -2720,7 +2723,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2751,7 +2754,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -2802,7 +2805,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2816,7 +2819,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2881,7 +2884,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3168,7 +3171,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3199,7 +3202,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -3291,7 +3294,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3322,7 +3325,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -3373,7 +3376,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3387,7 +3390,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="lv-LV"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3452,7 +3455,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="lv-LV"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3755,7 +3758,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3786,7 +3789,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277576"/>
@@ -3878,7 +3881,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="lv-LV"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3909,7 +3912,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="lv-LV"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488277248"/>
@@ -3960,7 +3963,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="lv-LV"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7130,6 +7133,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9E91EDFE-69A4-4DB5-9BEB-278FA52F3C99}" name="Table6" displayName="Table6" ref="A1:D61" totalsRowShown="0">
+  <autoFilter ref="A1:D61" xr:uid="{DEED746A-3EE2-4F95-862B-8D1FDA786B17}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1D358D9B-BDA9-4FAA-9527-A76EEDD11322}" name="Priority"/>
+    <tableColumn id="2" xr3:uid="{43410A99-A5DB-4E72-B8EF-85F1F7A20908}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{004396E5-C5A7-4451-9A9D-FB35C94CF099}" name="Time est. (hours)"/>
+    <tableColumn id="4" xr3:uid="{C11B94CA-8710-4830-8787-503C60BB7102}" name="Done"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78447A4E-CDB3-45EE-91A3-4EA22F56CF94}" name="Table2" displayName="Table2" ref="A1:J24" totalsRowShown="0">
   <autoFilter ref="A1:J24" xr:uid="{C94A59BC-04BB-4AF5-9E59-80489801E0B2}"/>
   <tableColumns count="10">
@@ -7148,7 +7164,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3FF0DD1C-4E49-4E7F-92CA-CB567AA3CB8E}" name="Table3" displayName="Table3" ref="A1:R34" totalsRowShown="0">
   <autoFilter ref="A1:R34" xr:uid="{A001DDB7-4D03-41B6-A7CC-449892123C18}"/>
   <tableColumns count="18">
@@ -7175,7 +7191,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6040D3C7-704D-4B34-9CD1-FCC83E772A66}" name="Table4" displayName="Table4" ref="A1:J35" totalsRowShown="0">
   <autoFilter ref="A1:J35" xr:uid="{ACD998EF-9F68-4272-9D9B-C9575E3BBCF2}"/>
   <tableColumns count="10">
@@ -7194,7 +7210,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{485FC9A2-2ECA-4867-B849-A896468FE32C}" name="Table1" displayName="Table1" ref="A1:L30" totalsRowShown="0">
   <autoFilter ref="A1:L30" xr:uid="{2C3F92BE-8B09-468B-934C-DB92BECE08EA}"/>
   <tableColumns count="12">
@@ -7215,23 +7231,23 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{69F42748-5731-45AD-AB2F-2D56CE6CE30F}" name="Tabula5" displayName="Tabula5" ref="A1:M22" totalsRowShown="0" dataDxfId="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{69F42748-5731-45AD-AB2F-2D56CE6CE30F}" name="Tabula5" displayName="Tabula5" ref="A1:M22" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="A1:M22" xr:uid="{53754D2A-1621-4F83-9B64-281BB9D7345E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{306EE1EA-B0B1-4175-8E88-A2B100506FAC}" name="Priority" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{4DF1E167-2B6E-4646-9E57-BBD0A536C003}" name="Work" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{FF972DE1-AB0B-4929-98A7-EF76BB4B4F75}" name="time-est." dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{E0A23C63-298C-4EE0-B937-0CE2842AEF13}" name="5.12.2017" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{06523220-F482-4E4F-80DF-AF0B07E8008D}" name="6.12.2017" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{F42B1C34-8E39-4DC4-812D-74DB150E1376}" name="7.12.2017" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{F8E2A858-D2A3-4E58-BF20-04FFF947CA18}" name="8.12.2017" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{591CA4B6-29BF-4E1C-B96F-D6DD1DF9437E}" name="9.12.2017" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{8FCC6452-56F4-4BEF-935B-9250EDB59435}" name="10.12.2017" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{14D28F79-F9A0-4876-8542-24D8499B8C69}" name="11.12.2017" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{DC40776A-5787-419C-BE3E-815487055AB1}" name="12.12.2017" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{A690D3DE-F147-4B4E-9360-A2B2A43A33D2}" name="13.12.2017" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{945433BC-B052-4280-81C3-8CFCBAC7FAF9}" name="Person" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{306EE1EA-B0B1-4175-8E88-A2B100506FAC}" name="Priority" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{4DF1E167-2B6E-4646-9E57-BBD0A536C003}" name="Work" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{FF972DE1-AB0B-4929-98A7-EF76BB4B4F75}" name="time-est." dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E0A23C63-298C-4EE0-B937-0CE2842AEF13}" name="5.12.2017" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{06523220-F482-4E4F-80DF-AF0B07E8008D}" name="6.12.2017" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{F42B1C34-8E39-4DC4-812D-74DB150E1376}" name="7.12.2017" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{F8E2A858-D2A3-4E58-BF20-04FFF947CA18}" name="8.12.2017" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{591CA4B6-29BF-4E1C-B96F-D6DD1DF9437E}" name="9.12.2017" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8FCC6452-56F4-4BEF-935B-9250EDB59435}" name="10.12.2017" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{14D28F79-F9A0-4876-8542-24D8499B8C69}" name="11.12.2017" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{DC40776A-5787-419C-BE3E-815487055AB1}" name="12.12.2017" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{A690D3DE-F147-4B4E-9360-A2B2A43A33D2}" name="13.12.2017" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{945433BC-B052-4280-81C3-8CFCBAC7FAF9}" name="Person" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7502,29 +7518,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView zoomScale="37" zoomScaleNormal="37" workbookViewId="0">
-      <selection activeCell="T56" sqref="T56"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
+      <c r="C1" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7532,13 +7550,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7546,13 +7564,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -7560,13 +7578,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7574,13 +7592,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7588,13 +7606,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -7602,13 +7620,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="1">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7616,13 +7634,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8">
         <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7630,13 +7648,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7644,13 +7662,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7658,13 +7676,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7672,13 +7690,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7686,13 +7704,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7700,13 +7718,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -7714,13 +7732,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7728,13 +7746,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7742,13 +7760,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7756,13 +7774,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7770,13 +7788,13 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7784,13 +7802,13 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7798,13 +7816,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -7812,13 +7830,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -7826,13 +7844,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -7840,13 +7858,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -7854,13 +7872,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -7868,13 +7886,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -7882,13 +7900,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -7896,13 +7914,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -7910,13 +7928,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -7924,13 +7942,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="1">
         <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -7938,13 +7956,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -7952,13 +7970,13 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1">
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -7966,13 +7984,13 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -7980,13 +7998,13 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="1">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -7994,13 +8012,13 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="1">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -8014,7 +8032,7 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -8022,13 +8040,13 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -8036,13 +8054,13 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -8050,13 +8068,13 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -8064,13 +8082,13 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -8078,13 +8096,13 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -8094,13 +8112,13 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="1">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -8110,13 +8128,13 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -8126,13 +8144,13 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -8142,13 +8160,13 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -8156,13 +8174,13 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -8172,13 +8190,13 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -8188,13 +8206,13 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -8204,13 +8222,13 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -8220,13 +8238,13 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="1">
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -8236,13 +8254,13 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C51" s="1">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -8252,13 +8270,13 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -8269,13 +8287,13 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" s="1">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -8286,13 +8304,13 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C54" s="1">
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F54" s="1"/>
       <c r="J54" s="1"/>
@@ -8302,13 +8320,13 @@
         <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" s="1">
         <v>3</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -8317,13 +8335,13 @@
         <v>3</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="1">
         <v>2</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -8332,13 +8350,13 @@
         <v>3</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="1">
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -8348,13 +8366,13 @@
         <v>3</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1">
         <v>6</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -8364,13 +8382,13 @@
         <v>3</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -8380,13 +8398,13 @@
         <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C60" s="1">
         <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -8396,13 +8414,13 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C61">
         <v>30</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
@@ -8522,6 +8540,9 @@
     <sortCondition ref="A28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -8556,22 +8577,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -8585,7 +8606,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1">
         <v>4</v>
@@ -8609,10 +8630,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8620,7 +8641,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -8644,10 +8665,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8655,7 +8676,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -8679,10 +8700,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8690,7 +8711,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
@@ -8714,10 +8735,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8725,7 +8746,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -8749,10 +8770,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8760,7 +8781,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1">
         <v>9</v>
@@ -8784,7 +8805,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8792,7 +8813,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -8816,7 +8837,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8824,7 +8845,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -8848,7 +8869,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8856,7 +8877,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -8880,7 +8901,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8888,7 +8909,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -8912,7 +8933,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8920,7 +8941,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1">
         <v>10</v>
@@ -8944,10 +8965,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8955,7 +8976,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -8979,10 +9000,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8990,7 +9011,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -9014,10 +9035,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9025,7 +9046,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -9049,7 +9070,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9057,7 +9078,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
@@ -9081,7 +9102,7 @@
         <v>3</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9089,7 +9110,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C17" s="1">
         <v>7</v>
@@ -9113,7 +9134,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9121,7 +9142,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C18" s="1">
         <v>4</v>
@@ -9145,7 +9166,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9153,7 +9174,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -9177,7 +9198,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9185,7 +9206,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="1">
         <v>10</v>
@@ -9209,7 +9230,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9217,7 +9238,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C21" s="1">
         <v>5</v>
@@ -9241,7 +9262,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9249,7 +9270,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -9273,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9281,7 +9302,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -9305,7 +9326,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9313,7 +9334,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -9337,12 +9358,12 @@
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25" s="1">
         <f>SUM(C2:C24)</f>
@@ -9371,7 +9392,7 @@
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" ref="D26:I26" si="1">SUM(D2:D24)</f>
@@ -9540,46 +9561,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>3</v>
@@ -9593,7 +9614,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
@@ -9641,7 +9662,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9649,7 +9670,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -9697,7 +9718,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9705,7 +9726,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -9753,7 +9774,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9761,7 +9782,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -9809,7 +9830,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9817,7 +9838,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -9865,7 +9886,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9873,7 +9894,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -9921,7 +9942,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9929,7 +9950,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -9977,7 +9998,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9985,7 +10006,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -10033,10 +10054,10 @@
         <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10044,7 +10065,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -10092,10 +10113,10 @@
         <v>0</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10103,7 +10124,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -10151,10 +10172,10 @@
         <v>0</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10162,7 +10183,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -10210,10 +10231,10 @@
         <v>0</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10221,7 +10242,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -10269,10 +10290,10 @@
         <v>0</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10280,7 +10301,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -10328,10 +10349,10 @@
         <v>0</v>
       </c>
       <c r="R14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10339,7 +10360,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -10387,10 +10408,10 @@
         <v>0</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10398,7 +10419,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
@@ -10446,10 +10467,10 @@
         <v>0</v>
       </c>
       <c r="R16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10457,7 +10478,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -10505,10 +10526,10 @@
         <v>0</v>
       </c>
       <c r="R17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10516,7 +10537,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -10564,10 +10585,10 @@
         <v>0</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10575,7 +10596,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -10623,10 +10644,10 @@
         <v>0</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10634,7 +10655,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -10682,10 +10703,10 @@
         <v>0</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10693,7 +10714,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -10741,10 +10762,10 @@
         <v>0</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S21" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10752,7 +10773,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
@@ -10800,10 +10821,10 @@
         <v>0</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10811,7 +10832,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -10859,10 +10880,10 @@
         <v>0</v>
       </c>
       <c r="R23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10870,7 +10891,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -10918,10 +10939,10 @@
         <v>0</v>
       </c>
       <c r="R24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10929,7 +10950,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -10977,10 +10998,10 @@
         <v>0</v>
       </c>
       <c r="R25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10988,7 +11009,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -11036,10 +11057,10 @@
         <v>0</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11047,7 +11068,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1">
         <v>6</v>
@@ -11095,10 +11116,10 @@
         <v>0</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11106,7 +11127,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -11154,7 +11175,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11162,7 +11183,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
@@ -11210,7 +11231,7 @@
         <v>0</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11218,7 +11239,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C30" s="1">
         <v>25</v>
@@ -11266,7 +11287,7 @@
         <v>0</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11274,7 +11295,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -11322,7 +11343,7 @@
         <v>0</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11330,7 +11351,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -11378,7 +11399,7 @@
         <v>0</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11386,7 +11407,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -11434,7 +11455,7 @@
         <v>0</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11442,7 +11463,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
@@ -11490,12 +11511,12 @@
         <v>0</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1">
         <f>SUM(C2:C34)</f>
@@ -11558,7 +11579,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36" s="1">
         <f>SUM(D2:D34)</f>
@@ -11890,22 +11911,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -11943,7 +11964,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11951,7 +11972,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -11975,7 +11996,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -11983,7 +12004,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -12007,7 +12028,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12015,7 +12036,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -12039,7 +12060,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12047,7 +12068,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -12071,7 +12092,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12079,7 +12100,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -12103,7 +12124,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12111,7 +12132,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1">
         <v>4</v>
@@ -12135,7 +12156,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12143,7 +12164,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -12167,7 +12188,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12175,7 +12196,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
@@ -12199,10 +12220,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12210,7 +12231,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -12234,10 +12255,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12245,7 +12266,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -12269,10 +12290,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12280,7 +12301,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -12304,10 +12325,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12315,7 +12336,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -12339,10 +12360,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12350,7 +12371,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -12374,10 +12395,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12385,7 +12406,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -12409,10 +12430,10 @@
         <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12420,7 +12441,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -12444,10 +12465,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12455,7 +12476,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -12479,10 +12500,10 @@
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12490,7 +12511,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -12514,10 +12535,10 @@
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12525,7 +12546,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -12549,10 +12570,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12560,7 +12581,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -12584,10 +12605,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12595,7 +12616,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -12619,10 +12640,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12630,7 +12651,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -12654,10 +12675,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12665,7 +12686,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -12689,7 +12710,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12697,7 +12718,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -12721,7 +12742,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12729,7 +12750,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
@@ -12753,7 +12774,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12761,7 +12782,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -12785,7 +12806,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12793,7 +12814,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -12817,7 +12838,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12825,7 +12846,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1">
         <v>9</v>
@@ -12849,7 +12870,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12857,7 +12878,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -12881,7 +12902,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12889,7 +12910,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -12913,7 +12934,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12921,7 +12942,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1">
         <v>4</v>
@@ -12945,7 +12966,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12953,7 +12974,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -12977,7 +12998,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12985,7 +13006,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C34" s="1">
         <v>18</v>
@@ -13009,7 +13030,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13017,7 +13038,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C35" s="1">
         <v>5</v>
@@ -13041,12 +13062,12 @@
         <v>0</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36" s="1">
         <f>SUM(C2:C35)</f>
@@ -13075,7 +13096,7 @@
     </row>
     <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" ref="D37:I37" si="1">SUM(D2:D35)</f>
@@ -13326,28 +13347,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -13361,7 +13382,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -13391,10 +13412,10 @@
         <v>3</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13402,7 +13423,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -13432,10 +13453,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13443,7 +13464,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -13473,10 +13494,10 @@
         <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13484,7 +13505,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -13514,10 +13535,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13525,7 +13546,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -13555,10 +13576,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13566,7 +13587,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -13596,10 +13617,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13607,7 +13628,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -13637,10 +13658,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13648,7 +13669,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -13678,10 +13699,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13689,7 +13710,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -13719,10 +13740,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13730,7 +13751,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -13760,10 +13781,10 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13771,7 +13792,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -13801,10 +13822,10 @@
         <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13812,7 +13833,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -13842,10 +13863,10 @@
         <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13853,7 +13874,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -13883,10 +13904,10 @@
         <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13894,7 +13915,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
@@ -13924,10 +13945,10 @@
         <v>0</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13935,7 +13956,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -13965,7 +13986,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13973,7 +13994,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -14003,7 +14024,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14011,7 +14032,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -14041,7 +14062,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14049,7 +14070,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -14079,7 +14100,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14087,7 +14108,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -14117,7 +14138,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14125,7 +14146,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -14155,7 +14176,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14163,7 +14184,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -14193,7 +14214,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14201,7 +14222,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="1">
         <v>4</v>
@@ -14231,7 +14252,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14239,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -14269,7 +14290,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14277,7 +14298,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
@@ -14307,7 +14328,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14315,7 +14336,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -14345,7 +14366,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14353,7 +14374,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -14383,7 +14404,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14391,7 +14412,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28" s="1">
         <v>25</v>
@@ -14421,7 +14442,7 @@
         <v>15</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14429,7 +14450,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1">
         <v>10</v>
@@ -14459,7 +14480,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14467,7 +14488,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
@@ -14497,12 +14518,12 @@
         <v>0</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D31" s="1">
         <f>SUM(C2:C30)</f>
@@ -14539,7 +14560,7 @@
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" ref="D32:K32" si="1">SUM(D2:D30)</f>
@@ -14663,7 +14684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3C4868-DA68-4B79-A75F-C29998123D8F}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -14692,31 +14713,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
@@ -14730,7 +14751,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C2" s="1">
         <v>6</v>
@@ -14763,7 +14784,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14771,7 +14792,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
@@ -14804,7 +14825,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14812,7 +14833,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
@@ -14845,7 +14866,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14853,7 +14874,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -14886,7 +14907,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14894,7 +14915,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -14927,7 +14948,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14935,7 +14956,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -14968,7 +14989,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -14976,7 +14997,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -15009,10 +15030,10 @@
         <v>0</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15020,7 +15041,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
@@ -15053,10 +15074,10 @@
         <v>0</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15064,7 +15085,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -15097,10 +15118,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15108,7 +15129,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -15141,10 +15162,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15152,7 +15173,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="1">
         <v>10</v>
@@ -15185,10 +15206,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15196,7 +15217,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -15229,10 +15250,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15240,7 +15261,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -15273,10 +15294,10 @@
         <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15284,7 +15305,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -15317,10 +15338,10 @@
         <v>0</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15328,7 +15349,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -15361,7 +15382,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15369,7 +15390,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -15402,7 +15423,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15410,7 +15431,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -15443,7 +15464,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15451,7 +15472,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -15484,7 +15505,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15492,7 +15513,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -15525,7 +15546,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15533,7 +15554,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C21" s="1">
         <v>20</v>
@@ -15566,7 +15587,7 @@
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15574,7 +15595,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="1">
         <v>4</v>
@@ -15607,12 +15628,12 @@
         <v>0</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(C2:C22)</f>
@@ -15653,7 +15674,7 @@
     </row>
     <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D24" s="1">
         <f>SUM(D2:D22)</f>

</xml_diff>